<commit_message>
roteiro de backend iniciado
</commit_message>
<xml_diff>
--- a/planejamento/cronograma-v2.xlsx
+++ b/planejamento/cronograma-v2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" firstSheet="6" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" firstSheet="6" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="CAPACIDADES" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="168">
   <si>
     <t>3. Desenvolver interfaces web utilizando frameworks</t>
   </si>
@@ -1387,10 +1387,6 @@
     <t>NoSQL</t>
   </si>
   <si>
-    <t>Apresentação Semestre
-Conceito Banco de Dados</t>
-  </si>
-  <si>
     <t>Início - Modelagem - Excel
 Apoio - exemplo-01.xlsx
 1:N
@@ -1402,9 +1398,6 @@
 Ajuste Conceitual - Lógico - Representação</t>
   </si>
   <si>
-    <t>ex: Filmes, Livros</t>
-  </si>
-  <si>
     <t>ex: Optus</t>
   </si>
   <si>
@@ -1412,16 +1405,6 @@
   </si>
   <si>
     <t>ex: PClinics, Locadora, E-Commerce</t>
-  </si>
-  <si>
-    <t>Início - DDL
-exemplo-ddl.sql
-01_roteiro_filmes.sql
-01_roteiro_livros.sql</t>
-  </si>
-  <si>
-    <t>RoteiroFilmes
-RoteiroLivros</t>
   </si>
   <si>
     <t>Desafio Ssolve - Documentação + Modelagem + DDL</t>
@@ -1432,11 +1415,6 @@
   <si>
     <t>Início - DML
 exemplo-dml.sql</t>
-  </si>
-  <si>
-    <t>RoteiroFilmes
-RoteiroLivros
-Optus</t>
   </si>
   <si>
     <t>Projeto - Gufos</t>
@@ -1455,6 +1433,35 @@
   </si>
   <si>
     <t>Procedures</t>
+  </si>
+  <si>
+    <t>RoteiroMusicas - SStop
+RoteiroLivros</t>
+  </si>
+  <si>
+    <t>ex: Musicas (sstop), Livros</t>
+  </si>
+  <si>
+    <t>Início - DDL
+exemplo-ddl.sql
+01_roteiro_sstop.sql
+01_roteiro_livros.sql</t>
+  </si>
+  <si>
+    <t>RoteiroMusicas - SStop
+RoteiroLivros
+Optus</t>
+  </si>
+  <si>
+    <t>Apresentação API</t>
+  </si>
+  <si>
+    <t>Apresentação Semestre
+Apresentação BD
+Conceito Banco de Dados</t>
+  </si>
+  <si>
+    <t>Desafio InLock</t>
   </si>
 </sst>
 </file>
@@ -31880,7 +31887,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CY69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="S1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="T18" sqref="T18:V30"/>
     </sheetView>
@@ -34350,7 +34357,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E103"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -34373,13 +34380,13 @@
         <v>141</v>
       </c>
       <c r="D1" s="426" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="E1" s="426" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="417" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="417" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="466" t="s">
         <v>142</v>
       </c>
@@ -34387,7 +34394,7 @@
         <v>43670</v>
       </c>
       <c r="C2" s="427" t="s">
-        <v>147</v>
+        <v>166</v>
       </c>
       <c r="D2" s="428"/>
       <c r="E2" s="428"/>
@@ -34407,10 +34414,10 @@
         <v>43672</v>
       </c>
       <c r="C4" s="430" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D4" s="431" t="s">
-        <v>150</v>
+        <v>162</v>
       </c>
       <c r="E4" s="431"/>
     </row>
@@ -34420,10 +34427,10 @@
         <v>43675</v>
       </c>
       <c r="C5" s="432" t="s">
+        <v>148</v>
+      </c>
+      <c r="D5" s="433" t="s">
         <v>149</v>
-      </c>
-      <c r="D5" s="433" t="s">
-        <v>151</v>
       </c>
       <c r="E5" s="433"/>
     </row>
@@ -34433,10 +34440,10 @@
         <v>43676</v>
       </c>
       <c r="C6" s="433" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D6" s="433" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E6" s="433"/>
     </row>
@@ -34446,10 +34453,10 @@
         <v>43677</v>
       </c>
       <c r="C7" s="432" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="D7" s="432" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="E7" s="433"/>
     </row>
@@ -34468,7 +34475,7 @@
         <v>43679</v>
       </c>
       <c r="C9" s="433" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D9" s="433"/>
       <c r="E9" s="433"/>
@@ -34479,10 +34486,10 @@
         <v>43682</v>
       </c>
       <c r="C10" s="430" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D10" s="430" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="E10" s="431"/>
     </row>
@@ -34492,10 +34499,10 @@
         <v>43683</v>
       </c>
       <c r="C11" s="431" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="D11" s="431" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="E11" s="431"/>
     </row>
@@ -34505,10 +34512,10 @@
         <v>43684</v>
       </c>
       <c r="C12" s="431" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="D12" s="431" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="E12" s="431"/>
     </row>
@@ -34527,7 +34534,7 @@
         <v>43686</v>
       </c>
       <c r="C14" s="431" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="D14" s="431"/>
       <c r="E14" s="431"/>
@@ -34538,11 +34545,11 @@
         <v>43689</v>
       </c>
       <c r="C15" s="433" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D15" s="433"/>
       <c r="E15" s="433" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="16" spans="1:5" s="420" customFormat="1" x14ac:dyDescent="0.25">
@@ -34551,7 +34558,7 @@
         <v>43690</v>
       </c>
       <c r="C16" s="433" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D16" s="433"/>
       <c r="E16" s="433"/>
@@ -34562,7 +34569,7 @@
         <v>43691</v>
       </c>
       <c r="C17" s="433" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D17" s="433"/>
       <c r="E17" s="433"/>
@@ -34582,7 +34589,7 @@
         <v>43693</v>
       </c>
       <c r="C19" s="433" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D19" s="434"/>
       <c r="E19" s="434"/>
@@ -34594,7 +34601,9 @@
       <c r="B20" s="402">
         <v>43696</v>
       </c>
-      <c r="C20" s="427"/>
+      <c r="C20" s="427" t="s">
+        <v>165</v>
+      </c>
       <c r="D20" s="428"/>
       <c r="E20" s="428"/>
     </row>
@@ -34630,7 +34639,9 @@
       <c r="B24" s="403">
         <v>43700</v>
       </c>
-      <c r="C24" s="431"/>
+      <c r="C24" s="431" t="s">
+        <v>167</v>
+      </c>
       <c r="D24" s="431"/>
       <c r="E24" s="431"/>
     </row>

</xml_diff>

<commit_message>
conteudo de react adicionado
</commit_message>
<xml_diff>
--- a/planejamento/cronograma-v2.xlsx
+++ b/planejamento/cronograma-v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erikv\Desktop\_Senai\senai-dev-2s2019\planejamento\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github_s\senai-dev-2s2019\planejamento\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD76B866-1697-479A-B42B-8C84118284CF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5A7523D-50D8-4221-BFDD-6CFA05EE9646}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11505" firstSheet="6" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="6" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CAPACIDADES" sheetId="1" r:id="rId1"/>
@@ -1582,22 +1582,12 @@
     <t>Interação - BackEnd/MongoDB</t>
   </si>
   <si>
-    <t>Introdução - Frameworks FrontEnd
-Introdução - React
-React - Base</t>
-  </si>
-  <si>
     <t>React
 Login</t>
   </si>
   <si>
     <t>React
 Eventos</t>
-  </si>
-  <si>
-    <t>React
-Categorias
-Componentes</t>
   </si>
   <si>
     <t>Desafio - Roman</t>
@@ -1608,6 +1598,17 @@
   <si>
     <t>ex: Optus, MicroManu</t>
   </si>
+  <si>
+    <t>Introdução - Frameworks FrontEnd
+Introdução - React
+React - Base
+React - Home</t>
+  </si>
+  <si>
+    <t>React - Home
+Categorias
+Componentes - Rodapé</t>
+  </si>
 </sst>
 </file>
 
@@ -1616,7 +1617,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m;@"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3685,208 +3686,208 @@
       <selection sqref="A1:A40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="96" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
         <v>35</v>
       </c>
@@ -3906,7 +3907,7 @@
       <selection pane="topRight" activeCell="BQ68" sqref="BQ68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="92" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.5703125" style="20" customWidth="1"/>
@@ -3944,7 +3945,7 @@
     <col min="108" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:119" s="61" customFormat="1" ht="15.75" thickBot="1">
+    <row r="1" spans="1:119" s="61" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="59"/>
       <c r="B1" s="447" t="s">
         <v>42</v>
@@ -4065,7 +4066,7 @@
       <c r="DB1" s="448"/>
       <c r="DC1" s="60"/>
     </row>
-    <row r="2" spans="1:119" s="24" customFormat="1">
+    <row r="2" spans="1:119" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>40</v>
       </c>
@@ -4400,7 +4401,7 @@
       <c r="DN2" s="23"/>
       <c r="DO2" s="23"/>
     </row>
-    <row r="3" spans="1:119" s="17" customFormat="1">
+    <row r="3" spans="1:119" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>5</v>
       </c>
@@ -4419,7 +4420,7 @@
       <c r="CL3" s="20"/>
       <c r="DC3" s="19"/>
     </row>
-    <row r="4" spans="1:119" s="17" customFormat="1">
+    <row r="4" spans="1:119" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>6</v>
       </c>
@@ -4438,7 +4439,7 @@
       <c r="CL4" s="20"/>
       <c r="DC4" s="19"/>
     </row>
-    <row r="5" spans="1:119" s="17" customFormat="1">
+    <row r="5" spans="1:119" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>8</v>
       </c>
@@ -4460,7 +4461,7 @@
       <c r="CL5" s="20"/>
       <c r="DC5" s="19"/>
     </row>
-    <row r="6" spans="1:119" s="17" customFormat="1">
+    <row r="6" spans="1:119" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>11</v>
       </c>
@@ -4482,7 +4483,7 @@
       <c r="CL6" s="20"/>
       <c r="DC6" s="19"/>
     </row>
-    <row r="7" spans="1:119" s="17" customFormat="1">
+    <row r="7" spans="1:119" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>7</v>
       </c>
@@ -4504,7 +4505,7 @@
       <c r="CL7" s="20"/>
       <c r="DC7" s="19"/>
     </row>
-    <row r="8" spans="1:119" s="17" customFormat="1">
+    <row r="8" spans="1:119" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>9</v>
       </c>
@@ -4526,7 +4527,7 @@
       <c r="CL8" s="20"/>
       <c r="DC8" s="19"/>
     </row>
-    <row r="9" spans="1:119" s="17" customFormat="1">
+    <row r="9" spans="1:119" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>13</v>
       </c>
@@ -4548,7 +4549,7 @@
       <c r="CL9" s="20"/>
       <c r="DC9" s="19"/>
     </row>
-    <row r="10" spans="1:119" s="17" customFormat="1">
+    <row r="10" spans="1:119" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>14</v>
       </c>
@@ -4570,7 +4571,7 @@
       <c r="CL10" s="20"/>
       <c r="DC10" s="19"/>
     </row>
-    <row r="11" spans="1:119" s="17" customFormat="1">
+    <row r="11" spans="1:119" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>10</v>
       </c>
@@ -4591,7 +4592,7 @@
       <c r="CL11" s="20"/>
       <c r="DC11" s="19"/>
     </row>
-    <row r="12" spans="1:119" s="17" customFormat="1">
+    <row r="12" spans="1:119" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>17</v>
       </c>
@@ -4611,7 +4612,7 @@
       <c r="CL12" s="20"/>
       <c r="DC12" s="19"/>
     </row>
-    <row r="13" spans="1:119" s="17" customFormat="1">
+    <row r="13" spans="1:119" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>15</v>
       </c>
@@ -4631,7 +4632,7 @@
       <c r="CL13" s="20"/>
       <c r="DC13" s="19"/>
     </row>
-    <row r="14" spans="1:119" s="17" customFormat="1">
+    <row r="14" spans="1:119" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
         <v>16</v>
       </c>
@@ -4652,7 +4653,7 @@
       <c r="CL14" s="20"/>
       <c r="DC14" s="19"/>
     </row>
-    <row r="15" spans="1:119" s="26" customFormat="1" ht="15.75" thickBot="1">
+    <row r="15" spans="1:119" s="26" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="30" t="s">
         <v>41</v>
       </c>
@@ -4676,7 +4677,7 @@
       <c r="CL15" s="25"/>
       <c r="DC15" s="32"/>
     </row>
-    <row r="16" spans="1:119" s="24" customFormat="1">
+    <row r="16" spans="1:119" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
         <v>18</v>
       </c>
@@ -4695,7 +4696,7 @@
       <c r="CL16" s="22"/>
       <c r="DC16" s="42"/>
     </row>
-    <row r="17" spans="1:16384" s="17" customFormat="1">
+    <row r="17" spans="1:16384" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>19</v>
       </c>
@@ -4714,7 +4715,7 @@
       <c r="CL17" s="20"/>
       <c r="DC17" s="19"/>
     </row>
-    <row r="18" spans="1:16384" s="17" customFormat="1">
+    <row r="18" spans="1:16384" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
         <v>21</v>
       </c>
@@ -4733,7 +4734,7 @@
       <c r="CL18" s="20"/>
       <c r="DC18" s="19"/>
     </row>
-    <row r="19" spans="1:16384" s="17" customFormat="1">
+    <row r="19" spans="1:16384" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="43" t="s">
         <v>62</v>
       </c>
@@ -4752,7 +4753,7 @@
       <c r="CL19" s="20"/>
       <c r="DC19" s="19"/>
     </row>
-    <row r="20" spans="1:16384" s="17" customFormat="1">
+    <row r="20" spans="1:16384" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
         <v>27</v>
       </c>
@@ -4775,7 +4776,7 @@
       <c r="CL20" s="20"/>
       <c r="DC20" s="19"/>
     </row>
-    <row r="21" spans="1:16384" s="17" customFormat="1">
+    <row r="21" spans="1:16384" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="43" t="s">
         <v>51</v>
       </c>
@@ -4796,7 +4797,7 @@
       <c r="CL21" s="20"/>
       <c r="DC21" s="19"/>
     </row>
-    <row r="22" spans="1:16384" s="17" customFormat="1">
+    <row r="22" spans="1:16384" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
         <v>22</v>
       </c>
@@ -4816,7 +4817,7 @@
       <c r="CL22" s="20"/>
       <c r="DC22" s="19"/>
     </row>
-    <row r="23" spans="1:16384" s="17" customFormat="1">
+    <row r="23" spans="1:16384" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
         <v>23</v>
       </c>
@@ -4835,7 +4836,7 @@
       <c r="CL23" s="20"/>
       <c r="DC23" s="19"/>
     </row>
-    <row r="24" spans="1:16384" s="17" customFormat="1">
+    <row r="24" spans="1:16384" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="43" t="s">
         <v>52</v>
       </c>
@@ -4859,7 +4860,7 @@
       <c r="CL24" s="20"/>
       <c r="DC24" s="19"/>
     </row>
-    <row r="25" spans="1:16384" s="17" customFormat="1">
+    <row r="25" spans="1:16384" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="43" t="s">
         <v>53</v>
       </c>
@@ -4882,7 +4883,7 @@
       <c r="CL25" s="20"/>
       <c r="DC25" s="19"/>
     </row>
-    <row r="26" spans="1:16384" s="17" customFormat="1">
+    <row r="26" spans="1:16384" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="43" t="s">
         <v>54</v>
       </c>
@@ -4905,7 +4906,7 @@
       <c r="CL26" s="20"/>
       <c r="DC26" s="19"/>
     </row>
-    <row r="27" spans="1:16384" s="17" customFormat="1">
+    <row r="27" spans="1:16384" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="43" t="s">
         <v>55</v>
       </c>
@@ -4930,7 +4931,7 @@
       <c r="CL27" s="20"/>
       <c r="DC27" s="19"/>
     </row>
-    <row r="28" spans="1:16384" s="17" customFormat="1">
+    <row r="28" spans="1:16384" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="43" t="s">
         <v>56</v>
       </c>
@@ -21316,7 +21317,7 @@
       <c r="XFC28" s="36"/>
       <c r="XFD28" s="36"/>
     </row>
-    <row r="29" spans="1:16384" s="17" customFormat="1">
+    <row r="29" spans="1:16384" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
         <v>57</v>
       </c>
@@ -21336,7 +21337,7 @@
       <c r="CL29" s="20"/>
       <c r="DC29" s="19"/>
     </row>
-    <row r="30" spans="1:16384" s="17" customFormat="1">
+    <row r="30" spans="1:16384" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="20" t="s">
         <v>58</v>
       </c>
@@ -21356,7 +21357,7 @@
       <c r="CL30" s="20"/>
       <c r="DC30" s="19"/>
     </row>
-    <row r="31" spans="1:16384" s="17" customFormat="1">
+    <row r="31" spans="1:16384" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
         <v>26</v>
       </c>
@@ -21375,7 +21376,7 @@
       <c r="CL31" s="20"/>
       <c r="DC31" s="19"/>
     </row>
-    <row r="32" spans="1:16384" s="17" customFormat="1">
+    <row r="32" spans="1:16384" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="43" t="s">
         <v>59</v>
       </c>
@@ -21395,7 +21396,7 @@
       <c r="CL32" s="20"/>
       <c r="DC32" s="19"/>
     </row>
-    <row r="33" spans="1:107" s="17" customFormat="1">
+    <row r="33" spans="1:107" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="43" t="s">
         <v>43</v>
       </c>
@@ -21415,7 +21416,7 @@
       <c r="CL33" s="20"/>
       <c r="DC33" s="19"/>
     </row>
-    <row r="34" spans="1:107" s="17" customFormat="1">
+    <row r="34" spans="1:107" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="43" t="s">
         <v>44</v>
       </c>
@@ -21437,7 +21438,7 @@
       <c r="CL34" s="20"/>
       <c r="DC34" s="19"/>
     </row>
-    <row r="35" spans="1:107" s="17" customFormat="1">
+    <row r="35" spans="1:107" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="43" t="s">
         <v>46</v>
       </c>
@@ -21457,7 +21458,7 @@
       <c r="CL35" s="20"/>
       <c r="DC35" s="19"/>
     </row>
-    <row r="36" spans="1:107" s="17" customFormat="1">
+    <row r="36" spans="1:107" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="43" t="s">
         <v>45</v>
       </c>
@@ -21479,7 +21480,7 @@
       <c r="CL36" s="20"/>
       <c r="DC36" s="19"/>
     </row>
-    <row r="37" spans="1:107" s="17" customFormat="1">
+    <row r="37" spans="1:107" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="43" t="s">
         <v>47</v>
       </c>
@@ -21499,7 +21500,7 @@
       <c r="CL37" s="20"/>
       <c r="DC37" s="19"/>
     </row>
-    <row r="38" spans="1:107" s="17" customFormat="1">
+    <row r="38" spans="1:107" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="43" t="s">
         <v>48</v>
       </c>
@@ -21519,7 +21520,7 @@
       <c r="CL38" s="20"/>
       <c r="DC38" s="19"/>
     </row>
-    <row r="39" spans="1:107" s="17" customFormat="1">
+    <row r="39" spans="1:107" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="43" t="s">
         <v>49</v>
       </c>
@@ -21539,7 +21540,7 @@
       <c r="CL39" s="20"/>
       <c r="DC39" s="19"/>
     </row>
-    <row r="40" spans="1:107" s="17" customFormat="1">
+    <row r="40" spans="1:107" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="43" t="s">
         <v>50</v>
       </c>
@@ -21559,7 +21560,7 @@
       <c r="CL40" s="20"/>
       <c r="DC40" s="19"/>
     </row>
-    <row r="41" spans="1:107" s="17" customFormat="1">
+    <row r="41" spans="1:107" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="43" t="s">
         <v>60</v>
       </c>
@@ -21580,7 +21581,7 @@
       <c r="CL41" s="20"/>
       <c r="DC41" s="19"/>
     </row>
-    <row r="42" spans="1:107" s="17" customFormat="1">
+    <row r="42" spans="1:107" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="43" t="s">
         <v>61</v>
       </c>
@@ -21601,7 +21602,7 @@
       <c r="CL42" s="20"/>
       <c r="DC42" s="19"/>
     </row>
-    <row r="43" spans="1:107" s="17" customFormat="1">
+    <row r="43" spans="1:107" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="43" t="s">
         <v>63</v>
       </c>
@@ -21624,7 +21625,7 @@
       <c r="CL43" s="20"/>
       <c r="DC43" s="19"/>
     </row>
-    <row r="44" spans="1:107" s="17" customFormat="1">
+    <row r="44" spans="1:107" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="20" t="s">
         <v>20</v>
       </c>
@@ -21651,7 +21652,7 @@
       <c r="CL44" s="20"/>
       <c r="DC44" s="19"/>
     </row>
-    <row r="45" spans="1:107" s="17" customFormat="1">
+    <row r="45" spans="1:107" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="20" t="s">
         <v>24</v>
       </c>
@@ -21671,7 +21672,7 @@
       <c r="CL45" s="20"/>
       <c r="DC45" s="19"/>
     </row>
-    <row r="46" spans="1:107" s="17" customFormat="1">
+    <row r="46" spans="1:107" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="20" t="s">
         <v>28</v>
       </c>
@@ -21695,7 +21696,7 @@
       <c r="CL46" s="20"/>
       <c r="DC46" s="19"/>
     </row>
-    <row r="47" spans="1:107" s="26" customFormat="1" ht="15.75" thickBot="1">
+    <row r="47" spans="1:107" s="26" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="30" t="s">
         <v>64</v>
       </c>
@@ -21731,7 +21732,7 @@
       <c r="CL47" s="25"/>
       <c r="DC47" s="32"/>
     </row>
-    <row r="48" spans="1:107" s="24" customFormat="1">
+    <row r="48" spans="1:107" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="22" t="s">
         <v>4</v>
       </c>
@@ -21754,7 +21755,7 @@
       <c r="CL48" s="22"/>
       <c r="DC48" s="42"/>
     </row>
-    <row r="49" spans="1:107" s="17" customFormat="1">
+    <row r="49" spans="1:107" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="20" t="s">
         <v>67</v>
       </c>
@@ -21775,7 +21776,7 @@
       <c r="CL49" s="20"/>
       <c r="DC49" s="19"/>
     </row>
-    <row r="50" spans="1:107" s="17" customFormat="1">
+    <row r="50" spans="1:107" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="20" t="s">
         <v>66</v>
       </c>
@@ -21799,7 +21800,7 @@
       <c r="CL50" s="20"/>
       <c r="DC50" s="19"/>
     </row>
-    <row r="51" spans="1:107" s="17" customFormat="1">
+    <row r="51" spans="1:107" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="20" t="s">
         <v>74</v>
       </c>
@@ -21824,7 +21825,7 @@
       <c r="CL51" s="20"/>
       <c r="DC51" s="19"/>
     </row>
-    <row r="52" spans="1:107" s="26" customFormat="1" ht="15.75" thickBot="1">
+    <row r="52" spans="1:107" s="26" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="30" t="s">
         <v>68</v>
       </c>
@@ -21851,7 +21852,7 @@
       <c r="CL52" s="25"/>
       <c r="DC52" s="32"/>
     </row>
-    <row r="53" spans="1:107" s="24" customFormat="1">
+    <row r="53" spans="1:107" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="22" t="s">
         <v>2</v>
       </c>
@@ -21877,7 +21878,7 @@
       <c r="CL53" s="22"/>
       <c r="DC53" s="42"/>
     </row>
-    <row r="54" spans="1:107" s="17" customFormat="1">
+    <row r="54" spans="1:107" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="20" t="s">
         <v>3</v>
       </c>
@@ -21903,7 +21904,7 @@
       <c r="CL54" s="20"/>
       <c r="DC54" s="19"/>
     </row>
-    <row r="55" spans="1:107" s="17" customFormat="1">
+    <row r="55" spans="1:107" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="20" t="s">
         <v>1</v>
       </c>
@@ -21927,7 +21928,7 @@
       <c r="CL55" s="20"/>
       <c r="DC55" s="19"/>
     </row>
-    <row r="56" spans="1:107" s="17" customFormat="1">
+    <row r="56" spans="1:107" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="20" t="s">
         <v>0</v>
       </c>
@@ -21956,7 +21957,7 @@
       <c r="CL56" s="20"/>
       <c r="DC56" s="19"/>
     </row>
-    <row r="57" spans="1:107" s="17" customFormat="1">
+    <row r="57" spans="1:107" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="43" t="s">
         <v>59</v>
       </c>
@@ -21984,7 +21985,7 @@
       <c r="CL57" s="20"/>
       <c r="DC57" s="19"/>
     </row>
-    <row r="58" spans="1:107" s="17" customFormat="1">
+    <row r="58" spans="1:107" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="43" t="s">
         <v>43</v>
       </c>
@@ -22012,7 +22013,7 @@
       <c r="CL58" s="20"/>
       <c r="DC58" s="19"/>
     </row>
-    <row r="59" spans="1:107" s="17" customFormat="1">
+    <row r="59" spans="1:107" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="43" t="s">
         <v>44</v>
       </c>
@@ -22040,7 +22041,7 @@
       <c r="CL59" s="20"/>
       <c r="DC59" s="19"/>
     </row>
-    <row r="60" spans="1:107" s="17" customFormat="1">
+    <row r="60" spans="1:107" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="43" t="s">
         <v>46</v>
       </c>
@@ -22067,7 +22068,7 @@
       <c r="CL60" s="20"/>
       <c r="DC60" s="19"/>
     </row>
-    <row r="61" spans="1:107" s="17" customFormat="1">
+    <row r="61" spans="1:107" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="43" t="s">
         <v>45</v>
       </c>
@@ -22094,7 +22095,7 @@
       <c r="CL61" s="20"/>
       <c r="DC61" s="19"/>
     </row>
-    <row r="62" spans="1:107" s="17" customFormat="1">
+    <row r="62" spans="1:107" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="43" t="s">
         <v>47</v>
       </c>
@@ -22121,7 +22122,7 @@
       <c r="CL62" s="20"/>
       <c r="DC62" s="19"/>
     </row>
-    <row r="63" spans="1:107" s="17" customFormat="1">
+    <row r="63" spans="1:107" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="43" t="s">
         <v>48</v>
       </c>
@@ -22149,7 +22150,7 @@
       <c r="CL63" s="20"/>
       <c r="DC63" s="19"/>
     </row>
-    <row r="64" spans="1:107" s="17" customFormat="1">
+    <row r="64" spans="1:107" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="43" t="s">
         <v>49</v>
       </c>
@@ -22177,7 +22178,7 @@
       <c r="CL64" s="20"/>
       <c r="DC64" s="19"/>
     </row>
-    <row r="65" spans="1:107" s="17" customFormat="1">
+    <row r="65" spans="1:107" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="43" t="s">
         <v>50</v>
       </c>
@@ -22205,7 +22206,7 @@
       <c r="CL65" s="20"/>
       <c r="DC65" s="19"/>
     </row>
-    <row r="66" spans="1:107" s="17" customFormat="1">
+    <row r="66" spans="1:107" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="43" t="s">
         <v>60</v>
       </c>
@@ -22233,7 +22234,7 @@
       <c r="CL66" s="20"/>
       <c r="DC66" s="19"/>
     </row>
-    <row r="67" spans="1:107" s="17" customFormat="1">
+    <row r="67" spans="1:107" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="43" t="s">
         <v>61</v>
       </c>
@@ -22260,7 +22261,7 @@
       <c r="CL67" s="20"/>
       <c r="DC67" s="19"/>
     </row>
-    <row r="68" spans="1:107" s="26" customFormat="1" ht="15.75" thickBot="1">
+    <row r="68" spans="1:107" s="26" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="30" t="s">
         <v>70</v>
       </c>
@@ -22288,7 +22289,7 @@
       <c r="CL68" s="25"/>
       <c r="DC68" s="32"/>
     </row>
-    <row r="69" spans="1:107" s="24" customFormat="1">
+    <row r="69" spans="1:107" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="50" t="s">
         <v>29</v>
       </c>
@@ -22309,7 +22310,7 @@
       <c r="CL69" s="22"/>
       <c r="DC69" s="42"/>
     </row>
-    <row r="70" spans="1:107" s="17" customFormat="1">
+    <row r="70" spans="1:107" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="45" t="s">
         <v>31</v>
       </c>
@@ -22330,7 +22331,7 @@
       <c r="CL70" s="20"/>
       <c r="DC70" s="19"/>
     </row>
-    <row r="71" spans="1:107" s="17" customFormat="1">
+    <row r="71" spans="1:107" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="51" t="s">
         <v>35</v>
       </c>
@@ -22352,7 +22353,7 @@
       <c r="CL71" s="20"/>
       <c r="DC71" s="19"/>
     </row>
-    <row r="72" spans="1:107" s="17" customFormat="1">
+    <row r="72" spans="1:107" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="45" t="s">
         <v>30</v>
       </c>
@@ -22373,7 +22374,7 @@
       <c r="CL72" s="20"/>
       <c r="DC72" s="19"/>
     </row>
-    <row r="73" spans="1:107" s="47" customFormat="1">
+    <row r="73" spans="1:107" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="45" t="s">
         <v>33</v>
       </c>
@@ -22394,7 +22395,7 @@
       <c r="CL73" s="46"/>
       <c r="DC73" s="49"/>
     </row>
-    <row r="74" spans="1:107" s="47" customFormat="1">
+    <row r="74" spans="1:107" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="46" t="s">
         <v>80</v>
       </c>
@@ -22416,7 +22417,7 @@
       <c r="CL74" s="46"/>
       <c r="DC74" s="49"/>
     </row>
-    <row r="75" spans="1:107" s="47" customFormat="1">
+    <row r="75" spans="1:107" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="43" t="s">
         <v>75</v>
       </c>
@@ -22438,7 +22439,7 @@
       <c r="CL75" s="46"/>
       <c r="DC75" s="49"/>
     </row>
-    <row r="76" spans="1:107" s="47" customFormat="1">
+    <row r="76" spans="1:107" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="43" t="s">
         <v>76</v>
       </c>
@@ -22460,7 +22461,7 @@
       <c r="CL76" s="46"/>
       <c r="DC76" s="49"/>
     </row>
-    <row r="77" spans="1:107" s="47" customFormat="1">
+    <row r="77" spans="1:107" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="43" t="s">
         <v>77</v>
       </c>
@@ -22482,7 +22483,7 @@
       <c r="CL77" s="46"/>
       <c r="DC77" s="49"/>
     </row>
-    <row r="78" spans="1:107" s="47" customFormat="1">
+    <row r="78" spans="1:107" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="43" t="s">
         <v>78</v>
       </c>
@@ -22504,7 +22505,7 @@
       <c r="CL78" s="46"/>
       <c r="DC78" s="49"/>
     </row>
-    <row r="79" spans="1:107" s="47" customFormat="1">
+    <row r="79" spans="1:107" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="43" t="s">
         <v>79</v>
       </c>
@@ -22526,7 +22527,7 @@
       <c r="CL79" s="46"/>
       <c r="DC79" s="49"/>
     </row>
-    <row r="80" spans="1:107" s="26" customFormat="1" ht="15.75" thickBot="1">
+    <row r="80" spans="1:107" s="26" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="30" t="s">
         <v>73</v>
       </c>
@@ -22557,7 +22558,7 @@
       <c r="CL80" s="62"/>
       <c r="DC80" s="32"/>
     </row>
-    <row r="81" spans="1:107" s="24" customFormat="1">
+    <row r="81" spans="1:107" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="22" t="s">
         <v>5</v>
       </c>
@@ -22579,7 +22580,7 @@
       <c r="CN81" s="44"/>
       <c r="DC81" s="42"/>
     </row>
-    <row r="82" spans="1:107" s="17" customFormat="1">
+    <row r="82" spans="1:107" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="20" t="s">
         <v>12</v>
       </c>
@@ -22600,7 +22601,7 @@
       <c r="CO82" s="21"/>
       <c r="DC82" s="19"/>
     </row>
-    <row r="83" spans="1:107" s="17" customFormat="1">
+    <row r="83" spans="1:107" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="20" t="s">
         <v>25</v>
       </c>
@@ -22621,7 +22622,7 @@
       <c r="CO83" s="21"/>
       <c r="DC83" s="19"/>
     </row>
-    <row r="84" spans="1:107" s="17" customFormat="1">
+    <row r="84" spans="1:107" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="20" t="s">
         <v>82</v>
       </c>
@@ -22642,7 +22643,7 @@
       <c r="CO84" s="21"/>
       <c r="DC84" s="19"/>
     </row>
-    <row r="85" spans="1:107" s="17" customFormat="1">
+    <row r="85" spans="1:107" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="20" t="s">
         <v>84</v>
       </c>
@@ -22666,7 +22667,7 @@
       <c r="CS85" s="21"/>
       <c r="DC85" s="19"/>
     </row>
-    <row r="86" spans="1:107" s="26" customFormat="1" ht="15.75" thickBot="1">
+    <row r="86" spans="1:107" s="26" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="30" t="s">
         <v>83</v>
       </c>
@@ -22720,7 +22721,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="7" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="6" width="4.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="13" width="3.85546875" bestFit="1" customWidth="1"/>
@@ -22734,7 +22735,7 @@
     <col min="96" max="100" width="5.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:100">
+    <row r="1" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A1" s="223">
         <v>43670</v>
       </c>
@@ -23051,7 +23052,7 @@
       <selection pane="topRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.28515625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="92" style="78" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.28515625" style="97"/>
@@ -23085,7 +23086,7 @@
     <col min="103" max="16384" width="8.28515625" style="63"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:102" s="100" customFormat="1">
+    <row r="1" spans="1:102" s="100" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="77"/>
       <c r="B1" s="459" t="s">
         <v>103</v>
@@ -23201,7 +23202,7 @@
       <c r="CW1" s="452"/>
       <c r="CX1" s="99"/>
     </row>
-    <row r="2" spans="1:102" s="107" customFormat="1" ht="15.75" thickBot="1">
+    <row r="2" spans="1:102" s="107" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="101" t="s">
         <v>94</v>
       </c>
@@ -23507,7 +23508,7 @@
       </c>
       <c r="CX2" s="208"/>
     </row>
-    <row r="3" spans="1:102" s="113" customFormat="1">
+    <row r="3" spans="1:102" s="113" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="108" t="s">
         <v>93</v>
       </c>
@@ -23613,7 +23614,7 @@
       <c r="CW3" s="111"/>
       <c r="CX3" s="209"/>
     </row>
-    <row r="4" spans="1:102" s="64" customFormat="1">
+    <row r="4" spans="1:102" s="64" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="79" t="s">
         <v>5</v>
       </c>
@@ -23636,7 +23637,7 @@
       <c r="CW4" s="87"/>
       <c r="CX4" s="71"/>
     </row>
-    <row r="5" spans="1:102" s="64" customFormat="1">
+    <row r="5" spans="1:102" s="64" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="79" t="s">
         <v>6</v>
       </c>
@@ -23659,7 +23660,7 @@
       <c r="CW5" s="87"/>
       <c r="CX5" s="71"/>
     </row>
-    <row r="6" spans="1:102" s="64" customFormat="1">
+    <row r="6" spans="1:102" s="64" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="79" t="s">
         <v>8</v>
       </c>
@@ -23685,7 +23686,7 @@
       <c r="CW6" s="87"/>
       <c r="CX6" s="71"/>
     </row>
-    <row r="7" spans="1:102" s="64" customFormat="1">
+    <row r="7" spans="1:102" s="64" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="79" t="s">
         <v>11</v>
       </c>
@@ -23711,7 +23712,7 @@
       <c r="CW7" s="87"/>
       <c r="CX7" s="71"/>
     </row>
-    <row r="8" spans="1:102" s="64" customFormat="1">
+    <row r="8" spans="1:102" s="64" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="79" t="s">
         <v>7</v>
       </c>
@@ -23737,7 +23738,7 @@
       <c r="CW8" s="87"/>
       <c r="CX8" s="71"/>
     </row>
-    <row r="9" spans="1:102" s="64" customFormat="1">
+    <row r="9" spans="1:102" s="64" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="79" t="s">
         <v>9</v>
       </c>
@@ -23763,7 +23764,7 @@
       <c r="CW9" s="87"/>
       <c r="CX9" s="71"/>
     </row>
-    <row r="10" spans="1:102" s="64" customFormat="1">
+    <row r="10" spans="1:102" s="64" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="79" t="s">
         <v>13</v>
       </c>
@@ -23789,7 +23790,7 @@
       <c r="CW10" s="87"/>
       <c r="CX10" s="71"/>
     </row>
-    <row r="11" spans="1:102" s="64" customFormat="1">
+    <row r="11" spans="1:102" s="64" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="79" t="s">
         <v>14</v>
       </c>
@@ -23815,7 +23816,7 @@
       <c r="CW11" s="87"/>
       <c r="CX11" s="71"/>
     </row>
-    <row r="12" spans="1:102" s="64" customFormat="1">
+    <row r="12" spans="1:102" s="64" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="79" t="s">
         <v>10</v>
       </c>
@@ -23839,7 +23840,7 @@
       <c r="CW12" s="87"/>
       <c r="CX12" s="71"/>
     </row>
-    <row r="13" spans="1:102" s="64" customFormat="1">
+    <row r="13" spans="1:102" s="64" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="79" t="s">
         <v>17</v>
       </c>
@@ -23863,7 +23864,7 @@
       <c r="CW13" s="87"/>
       <c r="CX13" s="71"/>
     </row>
-    <row r="14" spans="1:102" s="64" customFormat="1">
+    <row r="14" spans="1:102" s="64" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="79" t="s">
         <v>15</v>
       </c>
@@ -23887,7 +23888,7 @@
       <c r="CW14" s="87"/>
       <c r="CX14" s="71"/>
     </row>
-    <row r="15" spans="1:102" s="64" customFormat="1">
+    <row r="15" spans="1:102" s="64" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="79" t="s">
         <v>16</v>
       </c>
@@ -23912,7 +23913,7 @@
       <c r="CW15" s="87"/>
       <c r="CX15" s="71"/>
     </row>
-    <row r="16" spans="1:102" s="116" customFormat="1" ht="15.75" thickBot="1">
+    <row r="16" spans="1:102" s="116" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="114" t="s">
         <v>95</v>
       </c>
@@ -23940,7 +23941,7 @@
       <c r="CW16" s="166"/>
       <c r="CX16" s="118"/>
     </row>
-    <row r="17" spans="1:102" s="121" customFormat="1">
+    <row r="17" spans="1:102" s="121" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="119" t="s">
         <v>96</v>
       </c>
@@ -23963,7 +23964,7 @@
       <c r="CW17" s="122"/>
       <c r="CX17" s="123"/>
     </row>
-    <row r="18" spans="1:102" s="66" customFormat="1">
+    <row r="18" spans="1:102" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="80" t="s">
         <v>18</v>
       </c>
@@ -23985,7 +23986,7 @@
       <c r="CW18" s="90"/>
       <c r="CX18" s="72"/>
     </row>
-    <row r="19" spans="1:102" s="66" customFormat="1">
+    <row r="19" spans="1:102" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="80" t="s">
         <v>19</v>
       </c>
@@ -24007,7 +24008,7 @@
       <c r="CW19" s="90"/>
       <c r="CX19" s="72"/>
     </row>
-    <row r="20" spans="1:102" s="66" customFormat="1">
+    <row r="20" spans="1:102" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="80" t="s">
         <v>21</v>
       </c>
@@ -24030,7 +24031,7 @@
       <c r="CW20" s="90"/>
       <c r="CX20" s="72"/>
     </row>
-    <row r="21" spans="1:102" s="66" customFormat="1">
+    <row r="21" spans="1:102" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="80" t="s">
         <v>27</v>
       </c>
@@ -24058,7 +24059,7 @@
       <c r="CW21" s="90"/>
       <c r="CX21" s="72"/>
     </row>
-    <row r="22" spans="1:102" s="66" customFormat="1">
+    <row r="22" spans="1:102" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="80" t="s">
         <v>22</v>
       </c>
@@ -24082,7 +24083,7 @@
       <c r="CW22" s="90"/>
       <c r="CX22" s="72"/>
     </row>
-    <row r="23" spans="1:102" s="66" customFormat="1">
+    <row r="23" spans="1:102" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="80" t="s">
         <v>23</v>
       </c>
@@ -24110,7 +24111,7 @@
       <c r="CW23" s="90"/>
       <c r="CX23" s="72"/>
     </row>
-    <row r="24" spans="1:102" s="66" customFormat="1">
+    <row r="24" spans="1:102" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="80" t="s">
         <v>26</v>
       </c>
@@ -24132,7 +24133,7 @@
       <c r="CW24" s="90"/>
       <c r="CX24" s="72"/>
     </row>
-    <row r="25" spans="1:102" s="66" customFormat="1">
+    <row r="25" spans="1:102" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="81" t="s">
         <v>109</v>
       </c>
@@ -24155,7 +24156,7 @@
       <c r="CW25" s="90"/>
       <c r="CX25" s="72"/>
     </row>
-    <row r="26" spans="1:102" s="66" customFormat="1">
+    <row r="26" spans="1:102" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="81" t="s">
         <v>110</v>
       </c>
@@ -24178,7 +24179,7 @@
       <c r="CW26" s="90"/>
       <c r="CX26" s="72"/>
     </row>
-    <row r="27" spans="1:102" s="66" customFormat="1">
+    <row r="27" spans="1:102" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="81" t="s">
         <v>112</v>
       </c>
@@ -24201,7 +24202,7 @@
       <c r="CW27" s="90"/>
       <c r="CX27" s="72"/>
     </row>
-    <row r="28" spans="1:102" s="66" customFormat="1">
+    <row r="28" spans="1:102" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="81" t="s">
         <v>111</v>
       </c>
@@ -24224,7 +24225,7 @@
       <c r="CW28" s="90"/>
       <c r="CX28" s="72"/>
     </row>
-    <row r="29" spans="1:102" s="66" customFormat="1">
+    <row r="29" spans="1:102" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="81" t="s">
         <v>113</v>
       </c>
@@ -24247,7 +24248,7 @@
       <c r="CW29" s="90"/>
       <c r="CX29" s="72"/>
     </row>
-    <row r="30" spans="1:102" s="66" customFormat="1">
+    <row r="30" spans="1:102" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="81" t="s">
         <v>114</v>
       </c>
@@ -24270,7 +24271,7 @@
       <c r="CW30" s="90"/>
       <c r="CX30" s="72"/>
     </row>
-    <row r="31" spans="1:102" s="66" customFormat="1">
+    <row r="31" spans="1:102" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="80" t="s">
         <v>20</v>
       </c>
@@ -24293,7 +24294,7 @@
       <c r="CW31" s="90"/>
       <c r="CX31" s="72"/>
     </row>
-    <row r="32" spans="1:102" s="66" customFormat="1">
+    <row r="32" spans="1:102" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="80" t="s">
         <v>24</v>
       </c>
@@ -24316,7 +24317,7 @@
       <c r="CW32" s="90"/>
       <c r="CX32" s="72"/>
     </row>
-    <row r="33" spans="1:102" s="66" customFormat="1">
+    <row r="33" spans="1:102" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="80" t="s">
         <v>28</v>
       </c>
@@ -24339,7 +24340,7 @@
       <c r="CW33" s="90"/>
       <c r="CX33" s="72"/>
     </row>
-    <row r="34" spans="1:102" s="126" customFormat="1" ht="15.75" thickBot="1">
+    <row r="34" spans="1:102" s="126" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="124" t="s">
         <v>99</v>
       </c>
@@ -24369,7 +24370,7 @@
       <c r="CW34" s="127"/>
       <c r="CX34" s="128"/>
     </row>
-    <row r="35" spans="1:102" s="131" customFormat="1">
+    <row r="35" spans="1:102" s="131" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="129" t="s">
         <v>97</v>
       </c>
@@ -24392,7 +24393,7 @@
       <c r="CW35" s="132"/>
       <c r="CX35" s="133"/>
     </row>
-    <row r="36" spans="1:102" s="68" customFormat="1">
+    <row r="36" spans="1:102" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="82" t="s">
         <v>2</v>
       </c>
@@ -24413,7 +24414,7 @@
       <c r="CW36" s="92"/>
       <c r="CX36" s="73"/>
     </row>
-    <row r="37" spans="1:102" s="68" customFormat="1">
+    <row r="37" spans="1:102" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="82" t="s">
         <v>3</v>
       </c>
@@ -24436,7 +24437,7 @@
       <c r="CW37" s="92"/>
       <c r="CX37" s="73"/>
     </row>
-    <row r="38" spans="1:102" s="68" customFormat="1">
+    <row r="38" spans="1:102" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="82" t="s">
         <v>1</v>
       </c>
@@ -24458,7 +24459,7 @@
       <c r="CW38" s="92"/>
       <c r="CX38" s="73"/>
     </row>
-    <row r="39" spans="1:102" s="68" customFormat="1">
+    <row r="39" spans="1:102" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="82" t="s">
         <v>0</v>
       </c>
@@ -24479,7 +24480,7 @@
       <c r="CW39" s="92"/>
       <c r="CX39" s="73"/>
     </row>
-    <row r="40" spans="1:102" s="174" customFormat="1">
+    <row r="40" spans="1:102" s="174" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="172" t="s">
         <v>116</v>
       </c>
@@ -24501,7 +24502,7 @@
       <c r="CW40" s="175"/>
       <c r="CX40" s="176"/>
     </row>
-    <row r="41" spans="1:102" s="174" customFormat="1">
+    <row r="41" spans="1:102" s="174" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="172" t="s">
         <v>104</v>
       </c>
@@ -24523,7 +24524,7 @@
       <c r="CW41" s="175"/>
       <c r="CX41" s="176"/>
     </row>
-    <row r="42" spans="1:102" s="174" customFormat="1">
+    <row r="42" spans="1:102" s="174" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="172" t="s">
         <v>105</v>
       </c>
@@ -24545,7 +24546,7 @@
       <c r="CW42" s="175"/>
       <c r="CX42" s="176"/>
     </row>
-    <row r="43" spans="1:102" s="174" customFormat="1">
+    <row r="43" spans="1:102" s="174" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="172" t="s">
         <v>106</v>
       </c>
@@ -24567,7 +24568,7 @@
       <c r="CW43" s="175"/>
       <c r="CX43" s="176"/>
     </row>
-    <row r="44" spans="1:102" s="174" customFormat="1">
+    <row r="44" spans="1:102" s="174" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="172" t="s">
         <v>107</v>
       </c>
@@ -24589,7 +24590,7 @@
       <c r="CW44" s="175"/>
       <c r="CX44" s="176"/>
     </row>
-    <row r="45" spans="1:102" s="174" customFormat="1">
+    <row r="45" spans="1:102" s="174" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="172" t="s">
         <v>108</v>
       </c>
@@ -24611,7 +24612,7 @@
       <c r="CW45" s="175"/>
       <c r="CX45" s="176"/>
     </row>
-    <row r="46" spans="1:102" s="68" customFormat="1">
+    <row r="46" spans="1:102" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="82" t="s">
         <v>4</v>
       </c>
@@ -24634,7 +24635,7 @@
       <c r="CW46" s="92"/>
       <c r="CX46" s="73"/>
     </row>
-    <row r="47" spans="1:102" s="136" customFormat="1" ht="15.75" thickBot="1">
+    <row r="47" spans="1:102" s="136" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="134" t="s">
         <v>100</v>
       </c>
@@ -24669,7 +24670,7 @@
       <c r="CW47" s="137"/>
       <c r="CX47" s="138"/>
     </row>
-    <row r="48" spans="1:102" s="141" customFormat="1">
+    <row r="48" spans="1:102" s="141" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="139" t="s">
         <v>98</v>
       </c>
@@ -24692,7 +24693,7 @@
       <c r="CW48" s="142"/>
       <c r="CX48" s="143"/>
     </row>
-    <row r="49" spans="1:102" s="69" customFormat="1">
+    <row r="49" spans="1:102" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="83" t="s">
         <v>29</v>
       </c>
@@ -24714,7 +24715,7 @@
       <c r="CW49" s="94"/>
       <c r="CX49" s="74"/>
     </row>
-    <row r="50" spans="1:102" s="69" customFormat="1">
+    <row r="50" spans="1:102" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="83" t="s">
         <v>31</v>
       </c>
@@ -24735,7 +24736,7 @@
       <c r="CW50" s="94"/>
       <c r="CX50" s="74"/>
     </row>
-    <row r="51" spans="1:102" s="69" customFormat="1">
+    <row r="51" spans="1:102" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="83" t="s">
         <v>35</v>
       </c>
@@ -24757,7 +24758,7 @@
       <c r="CW51" s="94"/>
       <c r="CX51" s="74"/>
     </row>
-    <row r="52" spans="1:102" s="69" customFormat="1">
+    <row r="52" spans="1:102" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="83" t="s">
         <v>30</v>
       </c>
@@ -24779,7 +24780,7 @@
       <c r="CW52" s="94"/>
       <c r="CX52" s="74"/>
     </row>
-    <row r="53" spans="1:102" s="69" customFormat="1">
+    <row r="53" spans="1:102" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="83" t="s">
         <v>33</v>
       </c>
@@ -24801,7 +24802,7 @@
       <c r="CW53" s="94"/>
       <c r="CX53" s="74"/>
     </row>
-    <row r="54" spans="1:102" s="69" customFormat="1">
+    <row r="54" spans="1:102" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="83" t="s">
         <v>34</v>
       </c>
@@ -24823,7 +24824,7 @@
       <c r="CW54" s="94"/>
       <c r="CX54" s="74"/>
     </row>
-    <row r="55" spans="1:102" s="69" customFormat="1">
+    <row r="55" spans="1:102" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="83" t="s">
         <v>32</v>
       </c>
@@ -24844,7 +24845,7 @@
       <c r="CW55" s="94"/>
       <c r="CX55" s="74"/>
     </row>
-    <row r="56" spans="1:102" s="69" customFormat="1">
+    <row r="56" spans="1:102" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="181" t="s">
         <v>109</v>
       </c>
@@ -24866,7 +24867,7 @@
       <c r="CW56" s="94"/>
       <c r="CX56" s="74"/>
     </row>
-    <row r="57" spans="1:102" s="69" customFormat="1">
+    <row r="57" spans="1:102" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="181" t="s">
         <v>117</v>
       </c>
@@ -24889,7 +24890,7 @@
       <c r="CW57" s="94"/>
       <c r="CX57" s="74"/>
     </row>
-    <row r="58" spans="1:102" s="69" customFormat="1">
+    <row r="58" spans="1:102" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="181" t="s">
         <v>118</v>
       </c>
@@ -24911,7 +24912,7 @@
       <c r="CW58" s="94"/>
       <c r="CX58" s="74"/>
     </row>
-    <row r="59" spans="1:102" s="69" customFormat="1">
+    <row r="59" spans="1:102" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="181" t="s">
         <v>119</v>
       </c>
@@ -24933,7 +24934,7 @@
       <c r="CW59" s="94"/>
       <c r="CX59" s="74"/>
     </row>
-    <row r="60" spans="1:102" s="146" customFormat="1" ht="15.75" thickBot="1">
+    <row r="60" spans="1:102" s="146" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="144" t="s">
         <v>101</v>
       </c>
@@ -24970,7 +24971,7 @@
       <c r="CW60" s="147"/>
       <c r="CX60" s="148"/>
     </row>
-    <row r="61" spans="1:102" s="156" customFormat="1">
+    <row r="61" spans="1:102" s="156" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="154" t="s">
         <v>93</v>
       </c>
@@ -24993,7 +24994,7 @@
       <c r="CW61" s="157"/>
       <c r="CX61" s="158"/>
     </row>
-    <row r="62" spans="1:102" s="70" customFormat="1">
+    <row r="62" spans="1:102" s="70" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="85" t="s">
         <v>5</v>
       </c>
@@ -25017,7 +25018,7 @@
       <c r="CW62" s="96"/>
       <c r="CX62" s="75"/>
     </row>
-    <row r="63" spans="1:102" s="70" customFormat="1">
+    <row r="63" spans="1:102" s="70" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="85" t="s">
         <v>12</v>
       </c>
@@ -25041,7 +25042,7 @@
       <c r="CW63" s="96"/>
       <c r="CX63" s="75"/>
     </row>
-    <row r="64" spans="1:102" s="70" customFormat="1">
+    <row r="64" spans="1:102" s="70" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="84" t="s">
         <v>96</v>
       </c>
@@ -25064,7 +25065,7 @@
       <c r="CW64" s="96"/>
       <c r="CX64" s="75"/>
     </row>
-    <row r="65" spans="1:102" s="70" customFormat="1">
+    <row r="65" spans="1:102" s="70" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="85" t="s">
         <v>25</v>
       </c>
@@ -25088,7 +25089,7 @@
       <c r="CW65" s="96"/>
       <c r="CX65" s="75"/>
     </row>
-    <row r="66" spans="1:102" s="70" customFormat="1">
+    <row r="66" spans="1:102" s="70" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="85" t="s">
         <v>26</v>
       </c>
@@ -25112,7 +25113,7 @@
       <c r="CW66" s="96"/>
       <c r="CX66" s="75"/>
     </row>
-    <row r="67" spans="1:102" s="70" customFormat="1">
+    <row r="67" spans="1:102" s="70" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="84" t="s">
         <v>97</v>
       </c>
@@ -25135,7 +25136,7 @@
       <c r="CW67" s="96"/>
       <c r="CX67" s="75"/>
     </row>
-    <row r="68" spans="1:102" s="70" customFormat="1">
+    <row r="68" spans="1:102" s="70" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="85" t="s">
         <v>0</v>
       </c>
@@ -25160,7 +25161,7 @@
       <c r="CW68" s="96"/>
       <c r="CX68" s="75"/>
     </row>
-    <row r="69" spans="1:102" s="161" customFormat="1" ht="15.75" thickBot="1">
+    <row r="69" spans="1:102" s="161" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="159" t="s">
         <v>102</v>
       </c>
@@ -25188,7 +25189,7 @@
       <c r="CW69" s="162"/>
       <c r="CX69" s="163"/>
     </row>
-    <row r="70" spans="1:102" s="212" customFormat="1" ht="15.75" thickBot="1">
+    <row r="70" spans="1:102" s="212" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="210" t="s">
         <v>120</v>
       </c>
@@ -25213,7 +25214,7 @@
       </c>
       <c r="CX70" s="214"/>
     </row>
-    <row r="71" spans="1:102" s="151" customFormat="1">
+    <row r="71" spans="1:102" s="151" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="149"/>
       <c r="B71" s="150"/>
       <c r="P71" s="153"/>
@@ -25259,7 +25260,7 @@
       <selection pane="topRight" activeCell="DA49" sqref="DA49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.28515625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="92" style="78" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5" style="97" bestFit="1" customWidth="1"/>
@@ -25314,7 +25315,7 @@
     <col min="105" max="16384" width="8.28515625" style="63"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:104" s="100" customFormat="1">
+    <row r="1" spans="1:104" s="100" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="77"/>
       <c r="B1" s="459" t="s">
         <v>103</v>
@@ -25432,7 +25433,7 @@
       <c r="CY1" s="464"/>
       <c r="CZ1" s="99"/>
     </row>
-    <row r="2" spans="1:104" s="107" customFormat="1" ht="15.75" thickBot="1">
+    <row r="2" spans="1:104" s="107" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="101" t="s">
         <v>94</v>
       </c>
@@ -25744,7 +25745,7 @@
       </c>
       <c r="CZ2" s="208"/>
     </row>
-    <row r="3" spans="1:104" s="113" customFormat="1">
+    <row r="3" spans="1:104" s="113" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="108" t="s">
         <v>93</v>
       </c>
@@ -25851,7 +25852,7 @@
       <c r="CY3" s="269"/>
       <c r="CZ3" s="209"/>
     </row>
-    <row r="4" spans="1:104" s="64" customFormat="1">
+    <row r="4" spans="1:104" s="64" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="79" t="s">
         <v>5</v>
       </c>
@@ -25883,7 +25884,7 @@
       <c r="CY4" s="87"/>
       <c r="CZ4" s="71"/>
     </row>
-    <row r="5" spans="1:104" s="64" customFormat="1">
+    <row r="5" spans="1:104" s="64" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="79" t="s">
         <v>6</v>
       </c>
@@ -25915,7 +25916,7 @@
       <c r="CY5" s="87"/>
       <c r="CZ5" s="71"/>
     </row>
-    <row r="6" spans="1:104" s="64" customFormat="1">
+    <row r="6" spans="1:104" s="64" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="79" t="s">
         <v>8</v>
       </c>
@@ -25950,7 +25951,7 @@
       <c r="CY6" s="87"/>
       <c r="CZ6" s="71"/>
     </row>
-    <row r="7" spans="1:104" s="64" customFormat="1">
+    <row r="7" spans="1:104" s="64" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="79" t="s">
         <v>11</v>
       </c>
@@ -25987,7 +25988,7 @@
       <c r="CY7" s="87"/>
       <c r="CZ7" s="71"/>
     </row>
-    <row r="8" spans="1:104" s="64" customFormat="1">
+    <row r="8" spans="1:104" s="64" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="79" t="s">
         <v>7</v>
       </c>
@@ -26022,7 +26023,7 @@
       <c r="CY8" s="87"/>
       <c r="CZ8" s="71"/>
     </row>
-    <row r="9" spans="1:104" s="64" customFormat="1">
+    <row r="9" spans="1:104" s="64" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="79" t="s">
         <v>9</v>
       </c>
@@ -26057,7 +26058,7 @@
       <c r="CY9" s="87"/>
       <c r="CZ9" s="71"/>
     </row>
-    <row r="10" spans="1:104" s="64" customFormat="1">
+    <row r="10" spans="1:104" s="64" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="79" t="s">
         <v>13</v>
       </c>
@@ -26092,7 +26093,7 @@
       <c r="CY10" s="87"/>
       <c r="CZ10" s="71"/>
     </row>
-    <row r="11" spans="1:104" s="64" customFormat="1">
+    <row r="11" spans="1:104" s="64" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="79" t="s">
         <v>14</v>
       </c>
@@ -26127,7 +26128,7 @@
       <c r="CY11" s="87"/>
       <c r="CZ11" s="71"/>
     </row>
-    <row r="12" spans="1:104" s="64" customFormat="1">
+    <row r="12" spans="1:104" s="64" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="79" t="s">
         <v>10</v>
       </c>
@@ -26160,7 +26161,7 @@
       <c r="CY12" s="87"/>
       <c r="CZ12" s="71"/>
     </row>
-    <row r="13" spans="1:104" s="64" customFormat="1">
+    <row r="13" spans="1:104" s="64" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="79" t="s">
         <v>17</v>
       </c>
@@ -26193,7 +26194,7 @@
       <c r="CY13" s="87"/>
       <c r="CZ13" s="71"/>
     </row>
-    <row r="14" spans="1:104" s="64" customFormat="1">
+    <row r="14" spans="1:104" s="64" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="79" t="s">
         <v>15</v>
       </c>
@@ -26226,7 +26227,7 @@
       <c r="CY14" s="87"/>
       <c r="CZ14" s="71"/>
     </row>
-    <row r="15" spans="1:104" s="64" customFormat="1">
+    <row r="15" spans="1:104" s="64" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="79" t="s">
         <v>16</v>
       </c>
@@ -26260,7 +26261,7 @@
       <c r="CY15" s="87"/>
       <c r="CZ15" s="71"/>
     </row>
-    <row r="16" spans="1:104" s="116" customFormat="1" ht="15.75" thickBot="1">
+    <row r="16" spans="1:104" s="116" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="114" t="s">
         <v>95</v>
       </c>
@@ -26298,7 +26299,7 @@
       <c r="CY16" s="166"/>
       <c r="CZ16" s="118"/>
     </row>
-    <row r="17" spans="1:104" s="121" customFormat="1">
+    <row r="17" spans="1:104" s="121" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="119" t="s">
         <v>96</v>
       </c>
@@ -26329,7 +26330,7 @@
       <c r="CY17" s="122"/>
       <c r="CZ17" s="123"/>
     </row>
-    <row r="18" spans="1:104" s="66" customFormat="1">
+    <row r="18" spans="1:104" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="80" t="s">
         <v>18</v>
       </c>
@@ -26358,7 +26359,7 @@
       <c r="CY18" s="90"/>
       <c r="CZ18" s="72"/>
     </row>
-    <row r="19" spans="1:104" s="66" customFormat="1">
+    <row r="19" spans="1:104" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="80" t="s">
         <v>19</v>
       </c>
@@ -26388,7 +26389,7 @@
       <c r="CY19" s="90"/>
       <c r="CZ19" s="72"/>
     </row>
-    <row r="20" spans="1:104" s="66" customFormat="1">
+    <row r="20" spans="1:104" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="80" t="s">
         <v>21</v>
       </c>
@@ -26418,7 +26419,7 @@
       <c r="CY20" s="90"/>
       <c r="CZ20" s="72"/>
     </row>
-    <row r="21" spans="1:104" s="66" customFormat="1">
+    <row r="21" spans="1:104" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="80" t="s">
         <v>27</v>
       </c>
@@ -26453,7 +26454,7 @@
       <c r="CY21" s="90"/>
       <c r="CZ21" s="72"/>
     </row>
-    <row r="22" spans="1:104" s="66" customFormat="1">
+    <row r="22" spans="1:104" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="80" t="s">
         <v>22</v>
       </c>
@@ -26485,7 +26486,7 @@
       <c r="CY22" s="90"/>
       <c r="CZ22" s="72"/>
     </row>
-    <row r="23" spans="1:104" s="66" customFormat="1">
+    <row r="23" spans="1:104" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="80" t="s">
         <v>23</v>
       </c>
@@ -26520,7 +26521,7 @@
       <c r="CY23" s="90"/>
       <c r="CZ23" s="72"/>
     </row>
-    <row r="24" spans="1:104" s="66" customFormat="1">
+    <row r="24" spans="1:104" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="80" t="s">
         <v>26</v>
       </c>
@@ -26549,7 +26550,7 @@
       <c r="CY24" s="90"/>
       <c r="CZ24" s="72"/>
     </row>
-    <row r="25" spans="1:104" s="66" customFormat="1">
+    <row r="25" spans="1:104" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="81" t="s">
         <v>109</v>
       </c>
@@ -26579,7 +26580,7 @@
       <c r="CY25" s="90"/>
       <c r="CZ25" s="72"/>
     </row>
-    <row r="26" spans="1:104" s="66" customFormat="1">
+    <row r="26" spans="1:104" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="81" t="s">
         <v>110</v>
       </c>
@@ -26610,7 +26611,7 @@
       <c r="CY26" s="90"/>
       <c r="CZ26" s="72"/>
     </row>
-    <row r="27" spans="1:104" s="66" customFormat="1">
+    <row r="27" spans="1:104" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="81" t="s">
         <v>112</v>
       </c>
@@ -26640,7 +26641,7 @@
       <c r="CY27" s="90"/>
       <c r="CZ27" s="72"/>
     </row>
-    <row r="28" spans="1:104" s="66" customFormat="1">
+    <row r="28" spans="1:104" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="81" t="s">
         <v>111</v>
       </c>
@@ -26670,7 +26671,7 @@
       <c r="CY28" s="90"/>
       <c r="CZ28" s="72"/>
     </row>
-    <row r="29" spans="1:104" s="66" customFormat="1">
+    <row r="29" spans="1:104" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="81" t="s">
         <v>113</v>
       </c>
@@ -26700,7 +26701,7 @@
       <c r="CY29" s="90"/>
       <c r="CZ29" s="72"/>
     </row>
-    <row r="30" spans="1:104" s="66" customFormat="1">
+    <row r="30" spans="1:104" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="81" t="s">
         <v>114</v>
       </c>
@@ -26730,7 +26731,7 @@
       <c r="CY30" s="90"/>
       <c r="CZ30" s="72"/>
     </row>
-    <row r="31" spans="1:104" s="66" customFormat="1">
+    <row r="31" spans="1:104" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="80" t="s">
         <v>20</v>
       </c>
@@ -26760,7 +26761,7 @@
       <c r="CY31" s="90"/>
       <c r="CZ31" s="72"/>
     </row>
-    <row r="32" spans="1:104" s="66" customFormat="1">
+    <row r="32" spans="1:104" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="80" t="s">
         <v>24</v>
       </c>
@@ -26790,7 +26791,7 @@
       <c r="CY32" s="90"/>
       <c r="CZ32" s="72"/>
     </row>
-    <row r="33" spans="1:104" s="66" customFormat="1">
+    <row r="33" spans="1:104" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="80" t="s">
         <v>28</v>
       </c>
@@ -26821,7 +26822,7 @@
       <c r="CY33" s="90"/>
       <c r="CZ33" s="72"/>
     </row>
-    <row r="34" spans="1:104" s="126" customFormat="1" ht="15.75" thickBot="1">
+    <row r="34" spans="1:104" s="126" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="124" t="s">
         <v>99</v>
       </c>
@@ -26861,7 +26862,7 @@
       <c r="CY34" s="127"/>
       <c r="CZ34" s="128"/>
     </row>
-    <row r="35" spans="1:104" s="272" customFormat="1">
+    <row r="35" spans="1:104" s="272" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="270" t="s">
         <v>97</v>
       </c>
@@ -26891,7 +26892,7 @@
       <c r="CY35" s="274"/>
       <c r="CZ35" s="276"/>
     </row>
-    <row r="36" spans="1:104" s="68" customFormat="1">
+    <row r="36" spans="1:104" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="82" t="s">
         <v>2</v>
       </c>
@@ -26921,7 +26922,7 @@
       <c r="CY36" s="92"/>
       <c r="CZ36" s="73"/>
     </row>
-    <row r="37" spans="1:104" s="68" customFormat="1">
+    <row r="37" spans="1:104" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="82" t="s">
         <v>3</v>
       </c>
@@ -26953,7 +26954,7 @@
       <c r="CY37" s="92"/>
       <c r="CZ37" s="73"/>
     </row>
-    <row r="38" spans="1:104" s="68" customFormat="1">
+    <row r="38" spans="1:104" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="82" t="s">
         <v>1</v>
       </c>
@@ -26984,7 +26985,7 @@
       <c r="CY38" s="92"/>
       <c r="CZ38" s="73"/>
     </row>
-    <row r="39" spans="1:104" s="68" customFormat="1">
+    <row r="39" spans="1:104" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="82" t="s">
         <v>0</v>
       </c>
@@ -27014,7 +27015,7 @@
       <c r="CY39" s="92"/>
       <c r="CZ39" s="73"/>
     </row>
-    <row r="40" spans="1:104" s="174" customFormat="1">
+    <row r="40" spans="1:104" s="174" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="172" t="s">
         <v>116</v>
       </c>
@@ -27044,7 +27045,7 @@
       <c r="CY40" s="175"/>
       <c r="CZ40" s="176"/>
     </row>
-    <row r="41" spans="1:104" s="174" customFormat="1">
+    <row r="41" spans="1:104" s="174" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="172" t="s">
         <v>104</v>
       </c>
@@ -27074,7 +27075,7 @@
       <c r="CY41" s="175"/>
       <c r="CZ41" s="176"/>
     </row>
-    <row r="42" spans="1:104" s="174" customFormat="1">
+    <row r="42" spans="1:104" s="174" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="172" t="s">
         <v>105</v>
       </c>
@@ -27104,7 +27105,7 @@
       <c r="CY42" s="175"/>
       <c r="CZ42" s="176"/>
     </row>
-    <row r="43" spans="1:104" s="174" customFormat="1">
+    <row r="43" spans="1:104" s="174" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="172" t="s">
         <v>106</v>
       </c>
@@ -27134,7 +27135,7 @@
       <c r="CY43" s="175"/>
       <c r="CZ43" s="176"/>
     </row>
-    <row r="44" spans="1:104" s="174" customFormat="1">
+    <row r="44" spans="1:104" s="174" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="172" t="s">
         <v>107</v>
       </c>
@@ -27164,7 +27165,7 @@
       <c r="CY44" s="175"/>
       <c r="CZ44" s="176"/>
     </row>
-    <row r="45" spans="1:104" s="174" customFormat="1">
+    <row r="45" spans="1:104" s="174" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="172" t="s">
         <v>108</v>
       </c>
@@ -27194,7 +27195,7 @@
       <c r="CY45" s="175"/>
       <c r="CZ45" s="176"/>
     </row>
-    <row r="46" spans="1:104" s="68" customFormat="1">
+    <row r="46" spans="1:104" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="82" t="s">
         <v>4</v>
       </c>
@@ -27226,7 +27227,7 @@
       <c r="CY46" s="92"/>
       <c r="CZ46" s="73"/>
     </row>
-    <row r="47" spans="1:104" s="281" customFormat="1" ht="15.75" thickBot="1">
+    <row r="47" spans="1:104" s="281" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="279" t="s">
         <v>100</v>
       </c>
@@ -27270,7 +27271,7 @@
       <c r="CY47" s="283"/>
       <c r="CZ47" s="288"/>
     </row>
-    <row r="48" spans="1:104" s="141" customFormat="1">
+    <row r="48" spans="1:104" s="141" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="139" t="s">
         <v>98</v>
       </c>
@@ -27300,7 +27301,7 @@
       <c r="CY48" s="142"/>
       <c r="CZ48" s="143"/>
     </row>
-    <row r="49" spans="1:104" s="69" customFormat="1">
+    <row r="49" spans="1:104" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="83" t="s">
         <v>29</v>
       </c>
@@ -27329,7 +27330,7 @@
       <c r="CY49" s="94"/>
       <c r="CZ49" s="74"/>
     </row>
-    <row r="50" spans="1:104" s="69" customFormat="1">
+    <row r="50" spans="1:104" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="83" t="s">
         <v>31</v>
       </c>
@@ -27357,7 +27358,7 @@
       <c r="CY50" s="94"/>
       <c r="CZ50" s="74"/>
     </row>
-    <row r="51" spans="1:104" s="69" customFormat="1">
+    <row r="51" spans="1:104" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="83" t="s">
         <v>35</v>
       </c>
@@ -27386,7 +27387,7 @@
       <c r="CY51" s="94"/>
       <c r="CZ51" s="74"/>
     </row>
-    <row r="52" spans="1:104" s="69" customFormat="1">
+    <row r="52" spans="1:104" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="83" t="s">
         <v>30</v>
       </c>
@@ -27415,7 +27416,7 @@
       <c r="CY52" s="94"/>
       <c r="CZ52" s="74"/>
     </row>
-    <row r="53" spans="1:104" s="69" customFormat="1">
+    <row r="53" spans="1:104" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="83" t="s">
         <v>33</v>
       </c>
@@ -27444,7 +27445,7 @@
       <c r="CY53" s="94"/>
       <c r="CZ53" s="74"/>
     </row>
-    <row r="54" spans="1:104" s="69" customFormat="1">
+    <row r="54" spans="1:104" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="83" t="s">
         <v>34</v>
       </c>
@@ -27473,7 +27474,7 @@
       <c r="CY54" s="94"/>
       <c r="CZ54" s="74"/>
     </row>
-    <row r="55" spans="1:104" s="69" customFormat="1">
+    <row r="55" spans="1:104" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="83" t="s">
         <v>32</v>
       </c>
@@ -27501,7 +27502,7 @@
       <c r="CY55" s="94"/>
       <c r="CZ55" s="74"/>
     </row>
-    <row r="56" spans="1:104" s="69" customFormat="1">
+    <row r="56" spans="1:104" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="181" t="s">
         <v>109</v>
       </c>
@@ -27530,7 +27531,7 @@
       <c r="CY56" s="94"/>
       <c r="CZ56" s="74"/>
     </row>
-    <row r="57" spans="1:104" s="69" customFormat="1">
+    <row r="57" spans="1:104" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="181" t="s">
         <v>117</v>
       </c>
@@ -27560,7 +27561,7 @@
       <c r="CY57" s="94"/>
       <c r="CZ57" s="74"/>
     </row>
-    <row r="58" spans="1:104" s="69" customFormat="1">
+    <row r="58" spans="1:104" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="181" t="s">
         <v>118</v>
       </c>
@@ -27589,7 +27590,7 @@
       <c r="CY58" s="94"/>
       <c r="CZ58" s="74"/>
     </row>
-    <row r="59" spans="1:104" s="69" customFormat="1">
+    <row r="59" spans="1:104" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="181" t="s">
         <v>119</v>
       </c>
@@ -27618,7 +27619,7 @@
       <c r="CY59" s="94"/>
       <c r="CZ59" s="74"/>
     </row>
-    <row r="60" spans="1:104" s="146" customFormat="1" ht="15.75" thickBot="1">
+    <row r="60" spans="1:104" s="146" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="144" t="s">
         <v>101</v>
       </c>
@@ -27663,7 +27664,7 @@
       <c r="CY60" s="147"/>
       <c r="CZ60" s="148"/>
     </row>
-    <row r="61" spans="1:104" s="291" customFormat="1">
+    <row r="61" spans="1:104" s="291" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="289" t="s">
         <v>93</v>
       </c>
@@ -27695,7 +27696,7 @@
       <c r="CY61" s="293"/>
       <c r="CZ61" s="295"/>
     </row>
-    <row r="62" spans="1:104" s="70" customFormat="1">
+    <row r="62" spans="1:104" s="70" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="85" t="s">
         <v>5</v>
       </c>
@@ -27726,7 +27727,7 @@
       <c r="CY62" s="96"/>
       <c r="CZ62" s="75"/>
     </row>
-    <row r="63" spans="1:104" s="70" customFormat="1">
+    <row r="63" spans="1:104" s="70" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="85" t="s">
         <v>12</v>
       </c>
@@ -27757,7 +27758,7 @@
       <c r="CY63" s="96"/>
       <c r="CZ63" s="75"/>
     </row>
-    <row r="64" spans="1:104" s="70" customFormat="1">
+    <row r="64" spans="1:104" s="70" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="84" t="s">
         <v>96</v>
       </c>
@@ -27787,7 +27788,7 @@
       <c r="CY64" s="96"/>
       <c r="CZ64" s="75"/>
     </row>
-    <row r="65" spans="1:104" s="70" customFormat="1">
+    <row r="65" spans="1:104" s="70" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="85" t="s">
         <v>25</v>
       </c>
@@ -27818,7 +27819,7 @@
       <c r="CY65" s="96"/>
       <c r="CZ65" s="75"/>
     </row>
-    <row r="66" spans="1:104" s="70" customFormat="1">
+    <row r="66" spans="1:104" s="70" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="85" t="s">
         <v>26</v>
       </c>
@@ -27849,7 +27850,7 @@
       <c r="CY66" s="96"/>
       <c r="CZ66" s="75"/>
     </row>
-    <row r="67" spans="1:104" s="70" customFormat="1">
+    <row r="67" spans="1:104" s="70" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="84" t="s">
         <v>97</v>
       </c>
@@ -27879,7 +27880,7 @@
       <c r="CY67" s="96"/>
       <c r="CZ67" s="75"/>
     </row>
-    <row r="68" spans="1:104" s="70" customFormat="1">
+    <row r="68" spans="1:104" s="70" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="85" t="s">
         <v>0</v>
       </c>
@@ -27911,7 +27912,7 @@
       <c r="CY68" s="96"/>
       <c r="CZ68" s="75"/>
     </row>
-    <row r="69" spans="1:104" s="161" customFormat="1" ht="15.75" thickBot="1">
+    <row r="69" spans="1:104" s="161" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="159" t="s">
         <v>102</v>
       </c>
@@ -27944,7 +27945,7 @@
       <c r="CY69" s="162"/>
       <c r="CZ69" s="163"/>
     </row>
-    <row r="70" spans="1:104" s="212" customFormat="1" ht="15.75" thickBot="1">
+    <row r="70" spans="1:104" s="212" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="210" t="s">
         <v>120</v>
       </c>
@@ -27978,7 +27979,7 @@
       </c>
       <c r="CZ70" s="214"/>
     </row>
-    <row r="71" spans="1:104" s="151" customFormat="1">
+    <row r="71" spans="1:104" s="151" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="149"/>
       <c r="B71" s="150"/>
       <c r="P71" s="238"/>
@@ -28034,7 +28035,7 @@
       <selection pane="topRight" activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.28515625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="92" style="78" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5" style="97" bestFit="1" customWidth="1"/>
@@ -28112,7 +28113,7 @@
     <col min="105" max="16384" width="8.28515625" style="63"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:104" s="100" customFormat="1">
+    <row r="1" spans="1:104" s="100" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="77"/>
       <c r="B1" s="459" t="s">
         <v>103</v>
@@ -28230,7 +28231,7 @@
       <c r="CY1" s="464"/>
       <c r="CZ1" s="99"/>
     </row>
-    <row r="2" spans="1:104" s="107" customFormat="1" ht="15.75" thickBot="1">
+    <row r="2" spans="1:104" s="107" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="101" t="s">
         <v>94</v>
       </c>
@@ -28542,7 +28543,7 @@
       </c>
       <c r="CZ2" s="208"/>
     </row>
-    <row r="3" spans="1:104" s="113" customFormat="1">
+    <row r="3" spans="1:104" s="113" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="108" t="s">
         <v>93</v>
       </c>
@@ -28649,7 +28650,7 @@
       <c r="CY3" s="269"/>
       <c r="CZ3" s="209"/>
     </row>
-    <row r="4" spans="1:104" s="64" customFormat="1">
+    <row r="4" spans="1:104" s="64" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="79" t="s">
         <v>5</v>
       </c>
@@ -28699,7 +28700,7 @@
       <c r="CY4" s="87"/>
       <c r="CZ4" s="71"/>
     </row>
-    <row r="5" spans="1:104" s="64" customFormat="1">
+    <row r="5" spans="1:104" s="64" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="79" t="s">
         <v>6</v>
       </c>
@@ -28749,7 +28750,7 @@
       <c r="CY5" s="87"/>
       <c r="CZ5" s="71"/>
     </row>
-    <row r="6" spans="1:104" s="64" customFormat="1">
+    <row r="6" spans="1:104" s="64" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="79" t="s">
         <v>8</v>
       </c>
@@ -28801,7 +28802,7 @@
       <c r="CY6" s="87"/>
       <c r="CZ6" s="71"/>
     </row>
-    <row r="7" spans="1:104" s="64" customFormat="1">
+    <row r="7" spans="1:104" s="64" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="79" t="s">
         <v>11</v>
       </c>
@@ -28855,7 +28856,7 @@
       <c r="CY7" s="87"/>
       <c r="CZ7" s="71"/>
     </row>
-    <row r="8" spans="1:104" s="64" customFormat="1">
+    <row r="8" spans="1:104" s="64" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="79" t="s">
         <v>7</v>
       </c>
@@ -28907,7 +28908,7 @@
       <c r="CY8" s="87"/>
       <c r="CZ8" s="71"/>
     </row>
-    <row r="9" spans="1:104" s="64" customFormat="1">
+    <row r="9" spans="1:104" s="64" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="79" t="s">
         <v>9</v>
       </c>
@@ -28959,7 +28960,7 @@
       <c r="CY9" s="87"/>
       <c r="CZ9" s="71"/>
     </row>
-    <row r="10" spans="1:104" s="64" customFormat="1">
+    <row r="10" spans="1:104" s="64" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="79" t="s">
         <v>13</v>
       </c>
@@ -29011,7 +29012,7 @@
       <c r="CY10" s="87"/>
       <c r="CZ10" s="71"/>
     </row>
-    <row r="11" spans="1:104" s="64" customFormat="1">
+    <row r="11" spans="1:104" s="64" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="79" t="s">
         <v>14</v>
       </c>
@@ -29063,7 +29064,7 @@
       <c r="CY11" s="87"/>
       <c r="CZ11" s="71"/>
     </row>
-    <row r="12" spans="1:104" s="64" customFormat="1">
+    <row r="12" spans="1:104" s="64" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="79" t="s">
         <v>10</v>
       </c>
@@ -29114,7 +29115,7 @@
       <c r="CY12" s="87"/>
       <c r="CZ12" s="71"/>
     </row>
-    <row r="13" spans="1:104" s="64" customFormat="1">
+    <row r="13" spans="1:104" s="64" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="79" t="s">
         <v>17</v>
       </c>
@@ -29165,7 +29166,7 @@
       <c r="CY13" s="87"/>
       <c r="CZ13" s="71"/>
     </row>
-    <row r="14" spans="1:104" s="64" customFormat="1">
+    <row r="14" spans="1:104" s="64" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="79" t="s">
         <v>15</v>
       </c>
@@ -29216,7 +29217,7 @@
       <c r="CY14" s="87"/>
       <c r="CZ14" s="71"/>
     </row>
-    <row r="15" spans="1:104" s="64" customFormat="1">
+    <row r="15" spans="1:104" s="64" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="79" t="s">
         <v>16</v>
       </c>
@@ -29268,7 +29269,7 @@
       <c r="CY15" s="87"/>
       <c r="CZ15" s="71"/>
     </row>
-    <row r="16" spans="1:104" s="116" customFormat="1" ht="15.75" thickBot="1">
+    <row r="16" spans="1:104" s="116" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="114" t="s">
         <v>95</v>
       </c>
@@ -29323,7 +29324,7 @@
       <c r="CY16" s="166"/>
       <c r="CZ16" s="118"/>
     </row>
-    <row r="17" spans="1:104" s="121" customFormat="1">
+    <row r="17" spans="1:104" s="121" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="119" t="s">
         <v>96</v>
       </c>
@@ -29372,7 +29373,7 @@
       <c r="CY17" s="122"/>
       <c r="CZ17" s="123"/>
     </row>
-    <row r="18" spans="1:104" s="66" customFormat="1">
+    <row r="18" spans="1:104" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="80" t="s">
         <v>18</v>
       </c>
@@ -29419,7 +29420,7 @@
       <c r="CY18" s="90"/>
       <c r="CZ18" s="72"/>
     </row>
-    <row r="19" spans="1:104" s="66" customFormat="1">
+    <row r="19" spans="1:104" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="80" t="s">
         <v>19</v>
       </c>
@@ -29467,7 +29468,7 @@
       <c r="CY19" s="90"/>
       <c r="CZ19" s="72"/>
     </row>
-    <row r="20" spans="1:104" s="66" customFormat="1">
+    <row r="20" spans="1:104" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="80" t="s">
         <v>21</v>
       </c>
@@ -29515,7 +29516,7 @@
       <c r="CY20" s="90"/>
       <c r="CZ20" s="72"/>
     </row>
-    <row r="21" spans="1:104" s="66" customFormat="1">
+    <row r="21" spans="1:104" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="80" t="s">
         <v>27</v>
       </c>
@@ -29567,7 +29568,7 @@
       <c r="CY21" s="90"/>
       <c r="CZ21" s="72"/>
     </row>
-    <row r="22" spans="1:104" s="66" customFormat="1">
+    <row r="22" spans="1:104" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="80" t="s">
         <v>22</v>
       </c>
@@ -29616,7 +29617,7 @@
       <c r="CY22" s="90"/>
       <c r="CZ22" s="72"/>
     </row>
-    <row r="23" spans="1:104" s="66" customFormat="1">
+    <row r="23" spans="1:104" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="80" t="s">
         <v>23</v>
       </c>
@@ -29669,7 +29670,7 @@
       <c r="CY23" s="90"/>
       <c r="CZ23" s="72"/>
     </row>
-    <row r="24" spans="1:104" s="66" customFormat="1">
+    <row r="24" spans="1:104" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="80" t="s">
         <v>26</v>
       </c>
@@ -29716,7 +29717,7 @@
       <c r="CY24" s="90"/>
       <c r="CZ24" s="72"/>
     </row>
-    <row r="25" spans="1:104" s="66" customFormat="1">
+    <row r="25" spans="1:104" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="81" t="s">
         <v>109</v>
       </c>
@@ -29763,7 +29764,7 @@
       <c r="CY25" s="90"/>
       <c r="CZ25" s="72"/>
     </row>
-    <row r="26" spans="1:104" s="66" customFormat="1">
+    <row r="26" spans="1:104" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="81" t="s">
         <v>110</v>
       </c>
@@ -29812,7 +29813,7 @@
       <c r="CY26" s="90"/>
       <c r="CZ26" s="72"/>
     </row>
-    <row r="27" spans="1:104" s="66" customFormat="1">
+    <row r="27" spans="1:104" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="81" t="s">
         <v>112</v>
       </c>
@@ -29860,7 +29861,7 @@
       <c r="CY27" s="90"/>
       <c r="CZ27" s="72"/>
     </row>
-    <row r="28" spans="1:104" s="66" customFormat="1">
+    <row r="28" spans="1:104" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="81" t="s">
         <v>111</v>
       </c>
@@ -29908,7 +29909,7 @@
       <c r="CY28" s="90"/>
       <c r="CZ28" s="72"/>
     </row>
-    <row r="29" spans="1:104" s="66" customFormat="1">
+    <row r="29" spans="1:104" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="81" t="s">
         <v>113</v>
       </c>
@@ -29956,7 +29957,7 @@
       <c r="CY29" s="90"/>
       <c r="CZ29" s="72"/>
     </row>
-    <row r="30" spans="1:104" s="66" customFormat="1">
+    <row r="30" spans="1:104" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="81" t="s">
         <v>114</v>
       </c>
@@ -30004,7 +30005,7 @@
       <c r="CY30" s="90"/>
       <c r="CZ30" s="72"/>
     </row>
-    <row r="31" spans="1:104" s="66" customFormat="1">
+    <row r="31" spans="1:104" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="80" t="s">
         <v>20</v>
       </c>
@@ -30052,7 +30053,7 @@
       <c r="CY31" s="90"/>
       <c r="CZ31" s="72"/>
     </row>
-    <row r="32" spans="1:104" s="66" customFormat="1">
+    <row r="32" spans="1:104" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="80" t="s">
         <v>24</v>
       </c>
@@ -30100,7 +30101,7 @@
       <c r="CY32" s="90"/>
       <c r="CZ32" s="72"/>
     </row>
-    <row r="33" spans="1:104" s="66" customFormat="1">
+    <row r="33" spans="1:104" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="80" t="s">
         <v>28</v>
       </c>
@@ -30149,7 +30150,7 @@
       <c r="CY33" s="90"/>
       <c r="CZ33" s="72"/>
     </row>
-    <row r="34" spans="1:104" s="126" customFormat="1" ht="15.75" thickBot="1">
+    <row r="34" spans="1:104" s="126" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="124" t="s">
         <v>99</v>
       </c>
@@ -30205,7 +30206,7 @@
       <c r="CY34" s="127"/>
       <c r="CZ34" s="128"/>
     </row>
-    <row r="35" spans="1:104" s="272" customFormat="1">
+    <row r="35" spans="1:104" s="272" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="270" t="s">
         <v>97</v>
       </c>
@@ -30253,7 +30254,7 @@
       <c r="CY35" s="274"/>
       <c r="CZ35" s="276"/>
     </row>
-    <row r="36" spans="1:104" s="68" customFormat="1">
+    <row r="36" spans="1:104" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="82" t="s">
         <v>2</v>
       </c>
@@ -30302,7 +30303,7 @@
       <c r="CY36" s="92"/>
       <c r="CZ36" s="73"/>
     </row>
-    <row r="37" spans="1:104" s="68" customFormat="1">
+    <row r="37" spans="1:104" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="82" t="s">
         <v>3</v>
       </c>
@@ -30353,7 +30354,7 @@
       <c r="CY37" s="92"/>
       <c r="CZ37" s="73"/>
     </row>
-    <row r="38" spans="1:104" s="68" customFormat="1">
+    <row r="38" spans="1:104" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="82" t="s">
         <v>1</v>
       </c>
@@ -30402,7 +30403,7 @@
       <c r="CY38" s="92"/>
       <c r="CZ38" s="73"/>
     </row>
-    <row r="39" spans="1:104" s="68" customFormat="1">
+    <row r="39" spans="1:104" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="82" t="s">
         <v>0</v>
       </c>
@@ -30451,7 +30452,7 @@
       <c r="CY39" s="92"/>
       <c r="CZ39" s="73"/>
     </row>
-    <row r="40" spans="1:104" s="174" customFormat="1">
+    <row r="40" spans="1:104" s="174" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="172" t="s">
         <v>116</v>
       </c>
@@ -30500,7 +30501,7 @@
       <c r="CY40" s="175"/>
       <c r="CZ40" s="176"/>
     </row>
-    <row r="41" spans="1:104" s="174" customFormat="1">
+    <row r="41" spans="1:104" s="174" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="172" t="s">
         <v>104</v>
       </c>
@@ -30548,7 +30549,7 @@
       <c r="CY41" s="175"/>
       <c r="CZ41" s="176"/>
     </row>
-    <row r="42" spans="1:104" s="174" customFormat="1">
+    <row r="42" spans="1:104" s="174" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="172" t="s">
         <v>105</v>
       </c>
@@ -30596,7 +30597,7 @@
       <c r="CY42" s="175"/>
       <c r="CZ42" s="176"/>
     </row>
-    <row r="43" spans="1:104" s="174" customFormat="1">
+    <row r="43" spans="1:104" s="174" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="172" t="s">
         <v>106</v>
       </c>
@@ -30645,7 +30646,7 @@
       <c r="CY43" s="175"/>
       <c r="CZ43" s="176"/>
     </row>
-    <row r="44" spans="1:104" s="174" customFormat="1">
+    <row r="44" spans="1:104" s="174" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="172" t="s">
         <v>107</v>
       </c>
@@ -30694,7 +30695,7 @@
       <c r="CY44" s="175"/>
       <c r="CZ44" s="176"/>
     </row>
-    <row r="45" spans="1:104" s="174" customFormat="1">
+    <row r="45" spans="1:104" s="174" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="172" t="s">
         <v>108</v>
       </c>
@@ -30743,7 +30744,7 @@
       <c r="CY45" s="175"/>
       <c r="CZ45" s="176"/>
     </row>
-    <row r="46" spans="1:104" s="68" customFormat="1">
+    <row r="46" spans="1:104" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="82" t="s">
         <v>4</v>
       </c>
@@ -30794,7 +30795,7 @@
       <c r="CY46" s="92"/>
       <c r="CZ46" s="73"/>
     </row>
-    <row r="47" spans="1:104" s="281" customFormat="1" ht="15.75" thickBot="1">
+    <row r="47" spans="1:104" s="281" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="279" t="s">
         <v>100</v>
       </c>
@@ -30854,7 +30855,7 @@
       <c r="CY47" s="283"/>
       <c r="CZ47" s="288"/>
     </row>
-    <row r="48" spans="1:104" s="141" customFormat="1">
+    <row r="48" spans="1:104" s="141" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="139" t="s">
         <v>98</v>
       </c>
@@ -30902,7 +30903,7 @@
       <c r="CY48" s="142"/>
       <c r="CZ48" s="143"/>
     </row>
-    <row r="49" spans="1:104" s="69" customFormat="1">
+    <row r="49" spans="1:104" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="83" t="s">
         <v>29</v>
       </c>
@@ -30951,7 +30952,7 @@
       <c r="CY49" s="94"/>
       <c r="CZ49" s="74"/>
     </row>
-    <row r="50" spans="1:104" s="69" customFormat="1">
+    <row r="50" spans="1:104" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="83" t="s">
         <v>31</v>
       </c>
@@ -30999,7 +31000,7 @@
       <c r="CY50" s="94"/>
       <c r="CZ50" s="74"/>
     </row>
-    <row r="51" spans="1:104" s="69" customFormat="1">
+    <row r="51" spans="1:104" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="83" t="s">
         <v>35</v>
       </c>
@@ -31048,7 +31049,7 @@
       <c r="CY51" s="94"/>
       <c r="CZ51" s="74"/>
     </row>
-    <row r="52" spans="1:104" s="69" customFormat="1">
+    <row r="52" spans="1:104" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="83" t="s">
         <v>30</v>
       </c>
@@ -31096,7 +31097,7 @@
       <c r="CY52" s="94"/>
       <c r="CZ52" s="74"/>
     </row>
-    <row r="53" spans="1:104" s="69" customFormat="1">
+    <row r="53" spans="1:104" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="83" t="s">
         <v>33</v>
       </c>
@@ -31144,7 +31145,7 @@
       <c r="CY53" s="94"/>
       <c r="CZ53" s="74"/>
     </row>
-    <row r="54" spans="1:104" s="69" customFormat="1">
+    <row r="54" spans="1:104" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="83" t="s">
         <v>34</v>
       </c>
@@ -31193,7 +31194,7 @@
       <c r="CY54" s="94"/>
       <c r="CZ54" s="74"/>
     </row>
-    <row r="55" spans="1:104" s="69" customFormat="1">
+    <row r="55" spans="1:104" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="83" t="s">
         <v>32</v>
       </c>
@@ -31241,7 +31242,7 @@
       <c r="CY55" s="94"/>
       <c r="CZ55" s="74"/>
     </row>
-    <row r="56" spans="1:104" s="69" customFormat="1">
+    <row r="56" spans="1:104" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="181" t="s">
         <v>109</v>
       </c>
@@ -31290,7 +31291,7 @@
       <c r="CY56" s="94"/>
       <c r="CZ56" s="74"/>
     </row>
-    <row r="57" spans="1:104" s="69" customFormat="1">
+    <row r="57" spans="1:104" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="181" t="s">
         <v>117</v>
       </c>
@@ -31340,7 +31341,7 @@
       <c r="CY57" s="94"/>
       <c r="CZ57" s="74"/>
     </row>
-    <row r="58" spans="1:104" s="69" customFormat="1">
+    <row r="58" spans="1:104" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="181" t="s">
         <v>118</v>
       </c>
@@ -31389,7 +31390,7 @@
       <c r="CY58" s="94"/>
       <c r="CZ58" s="74"/>
     </row>
-    <row r="59" spans="1:104" s="69" customFormat="1">
+    <row r="59" spans="1:104" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="181" t="s">
         <v>119</v>
       </c>
@@ -31438,7 +31439,7 @@
       <c r="CY59" s="94"/>
       <c r="CZ59" s="74"/>
     </row>
-    <row r="60" spans="1:104" s="146" customFormat="1" ht="15.75" thickBot="1">
+    <row r="60" spans="1:104" s="146" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="144" t="s">
         <v>101</v>
       </c>
@@ -31499,7 +31500,7 @@
       <c r="CY60" s="147"/>
       <c r="CZ60" s="148"/>
     </row>
-    <row r="61" spans="1:104" s="291" customFormat="1">
+    <row r="61" spans="1:104" s="291" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="289" t="s">
         <v>93</v>
       </c>
@@ -31549,7 +31550,7 @@
       <c r="CY61" s="293"/>
       <c r="CZ61" s="295"/>
     </row>
-    <row r="62" spans="1:104" s="70" customFormat="1">
+    <row r="62" spans="1:104" s="70" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="85" t="s">
         <v>5</v>
       </c>
@@ -31598,7 +31599,7 @@
       <c r="CY62" s="96"/>
       <c r="CZ62" s="75"/>
     </row>
-    <row r="63" spans="1:104" s="70" customFormat="1">
+    <row r="63" spans="1:104" s="70" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="85" t="s">
         <v>12</v>
       </c>
@@ -31647,7 +31648,7 @@
       <c r="CY63" s="96"/>
       <c r="CZ63" s="75"/>
     </row>
-    <row r="64" spans="1:104" s="70" customFormat="1">
+    <row r="64" spans="1:104" s="70" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="84" t="s">
         <v>96</v>
       </c>
@@ -31695,7 +31696,7 @@
       <c r="CY64" s="96"/>
       <c r="CZ64" s="75"/>
     </row>
-    <row r="65" spans="1:104" s="70" customFormat="1">
+    <row r="65" spans="1:104" s="70" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="85" t="s">
         <v>25</v>
       </c>
@@ -31743,7 +31744,7 @@
       <c r="CY65" s="96"/>
       <c r="CZ65" s="75"/>
     </row>
-    <row r="66" spans="1:104" s="70" customFormat="1">
+    <row r="66" spans="1:104" s="70" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="85" t="s">
         <v>26</v>
       </c>
@@ -31792,7 +31793,7 @@
       <c r="CY66" s="96"/>
       <c r="CZ66" s="75"/>
     </row>
-    <row r="67" spans="1:104" s="70" customFormat="1">
+    <row r="67" spans="1:104" s="70" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="84" t="s">
         <v>97</v>
       </c>
@@ -31840,7 +31841,7 @@
       <c r="CY67" s="96"/>
       <c r="CZ67" s="75"/>
     </row>
-    <row r="68" spans="1:104" s="70" customFormat="1">
+    <row r="68" spans="1:104" s="70" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="85" t="s">
         <v>0</v>
       </c>
@@ -31889,7 +31890,7 @@
       <c r="CY68" s="96"/>
       <c r="CZ68" s="75"/>
     </row>
-    <row r="69" spans="1:104" s="161" customFormat="1" ht="15.75" thickBot="1">
+    <row r="69" spans="1:104" s="161" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="159" t="s">
         <v>102</v>
       </c>
@@ -31939,7 +31940,7 @@
       <c r="CY69" s="162"/>
       <c r="CZ69" s="163"/>
     </row>
-    <row r="70" spans="1:104" s="212" customFormat="1" ht="15.75" thickBot="1">
+    <row r="70" spans="1:104" s="212" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="210" t="s">
         <v>120</v>
       </c>
@@ -31991,7 +31992,7 @@
       </c>
       <c r="CZ70" s="214"/>
     </row>
-    <row r="71" spans="1:104" s="151" customFormat="1">
+    <row r="71" spans="1:104" s="151" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="149"/>
       <c r="B71" s="150"/>
       <c r="C71" s="304"/>
@@ -32060,12 +32061,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:CY69"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScale="98" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A18" zoomScale="98" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="AN1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="CQ67" sqref="CQ67:CT67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="6.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="102.28515625" style="78" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.5703125" style="361"/>
@@ -32113,7 +32114,7 @@
     <col min="100" max="16384" width="6.5703125" style="334"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:103" s="350" customFormat="1">
+    <row r="1" spans="1:103" s="350" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="77"/>
       <c r="B1" s="351"/>
       <c r="C1" s="344"/>
@@ -32138,7 +32139,7 @@
       <c r="CP1" s="344"/>
       <c r="CU1" s="344"/>
     </row>
-    <row r="2" spans="1:103" s="107" customFormat="1" ht="15.75" thickBot="1">
+    <row r="2" spans="1:103" s="107" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="101" t="s">
         <v>94</v>
       </c>
@@ -32449,7 +32450,7 @@
         <v>43817</v>
       </c>
     </row>
-    <row r="3" spans="1:103" s="343" customFormat="1">
+    <row r="3" spans="1:103" s="343" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="108" t="s">
         <v>93</v>
       </c>
@@ -32479,7 +32480,7 @@
       <c r="CP3" s="344"/>
       <c r="CU3" s="344"/>
     </row>
-    <row r="4" spans="1:103" s="332" customFormat="1">
+    <row r="4" spans="1:103" s="332" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="79" t="s">
         <v>5</v>
       </c>
@@ -32509,7 +32510,7 @@
       <c r="CP4" s="333"/>
       <c r="CU4" s="333"/>
     </row>
-    <row r="5" spans="1:103" s="332" customFormat="1">
+    <row r="5" spans="1:103" s="332" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="79" t="s">
         <v>6</v>
       </c>
@@ -32539,7 +32540,7 @@
       <c r="CP5" s="333"/>
       <c r="CU5" s="333"/>
     </row>
-    <row r="6" spans="1:103" s="332" customFormat="1">
+    <row r="6" spans="1:103" s="332" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="79" t="s">
         <v>8</v>
       </c>
@@ -32575,7 +32576,7 @@
       <c r="CP6" s="333"/>
       <c r="CU6" s="333"/>
     </row>
-    <row r="7" spans="1:103" s="332" customFormat="1">
+    <row r="7" spans="1:103" s="332" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="79" t="s">
         <v>11</v>
       </c>
@@ -32609,7 +32610,7 @@
       <c r="CP7" s="333"/>
       <c r="CU7" s="333"/>
     </row>
-    <row r="8" spans="1:103" s="332" customFormat="1">
+    <row r="8" spans="1:103" s="332" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="79" t="s">
         <v>7</v>
       </c>
@@ -32644,7 +32645,7 @@
       <c r="CP8" s="333"/>
       <c r="CU8" s="333"/>
     </row>
-    <row r="9" spans="1:103" s="332" customFormat="1">
+    <row r="9" spans="1:103" s="332" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="79" t="s">
         <v>9</v>
       </c>
@@ -32678,7 +32679,7 @@
       <c r="CP9" s="333"/>
       <c r="CU9" s="333"/>
     </row>
-    <row r="10" spans="1:103" s="332" customFormat="1">
+    <row r="10" spans="1:103" s="332" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="79" t="s">
         <v>13</v>
       </c>
@@ -32712,7 +32713,7 @@
       <c r="CP10" s="333"/>
       <c r="CU10" s="333"/>
     </row>
-    <row r="11" spans="1:103" s="332" customFormat="1">
+    <row r="11" spans="1:103" s="332" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="79" t="s">
         <v>14</v>
       </c>
@@ -32747,7 +32748,7 @@
       <c r="CP11" s="333"/>
       <c r="CU11" s="333"/>
     </row>
-    <row r="12" spans="1:103" s="332" customFormat="1">
+    <row r="12" spans="1:103" s="332" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="79" t="s">
         <v>10</v>
       </c>
@@ -32781,7 +32782,7 @@
       <c r="CP12" s="333"/>
       <c r="CU12" s="333"/>
     </row>
-    <row r="13" spans="1:103" s="332" customFormat="1">
+    <row r="13" spans="1:103" s="332" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="79" t="s">
         <v>17</v>
       </c>
@@ -32815,7 +32816,7 @@
       <c r="CP13" s="333"/>
       <c r="CU13" s="333"/>
     </row>
-    <row r="14" spans="1:103" s="332" customFormat="1">
+    <row r="14" spans="1:103" s="332" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="79" t="s">
         <v>15</v>
       </c>
@@ -32846,7 +32847,7 @@
       <c r="CP14" s="333"/>
       <c r="CU14" s="333"/>
     </row>
-    <row r="15" spans="1:103" s="332" customFormat="1">
+    <row r="15" spans="1:103" s="332" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="79" t="s">
         <v>16</v>
       </c>
@@ -32877,7 +32878,7 @@
       <c r="CP15" s="333"/>
       <c r="CU15" s="333"/>
     </row>
-    <row r="16" spans="1:103" s="346" customFormat="1" ht="15.75" thickBot="1">
+    <row r="16" spans="1:103" s="346" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="114" t="s">
         <v>95</v>
       </c>
@@ -32909,7 +32910,7 @@
       <c r="CP16" s="347"/>
       <c r="CU16" s="347"/>
     </row>
-    <row r="17" spans="1:99" s="363" customFormat="1">
+    <row r="17" spans="1:99" s="363" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="119" t="s">
         <v>96</v>
       </c>
@@ -32936,7 +32937,7 @@
       <c r="CP17" s="344"/>
       <c r="CU17" s="344"/>
     </row>
-    <row r="18" spans="1:99" s="337" customFormat="1">
+    <row r="18" spans="1:99" s="337" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="80" t="s">
         <v>18</v>
       </c>
@@ -32967,7 +32968,7 @@
       <c r="CP18" s="333"/>
       <c r="CU18" s="333"/>
     </row>
-    <row r="19" spans="1:99" s="337" customFormat="1">
+    <row r="19" spans="1:99" s="337" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="80" t="s">
         <v>19</v>
       </c>
@@ -32998,7 +32999,7 @@
       <c r="CP19" s="333"/>
       <c r="CU19" s="333"/>
     </row>
-    <row r="20" spans="1:99" s="337" customFormat="1">
+    <row r="20" spans="1:99" s="337" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="80" t="s">
         <v>21</v>
       </c>
@@ -33026,7 +33027,7 @@
       <c r="CP20" s="333"/>
       <c r="CU20" s="333"/>
     </row>
-    <row r="21" spans="1:99" s="337" customFormat="1">
+    <row r="21" spans="1:99" s="337" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="80" t="s">
         <v>27</v>
       </c>
@@ -33054,7 +33055,7 @@
       <c r="CP21" s="333"/>
       <c r="CU21" s="333"/>
     </row>
-    <row r="22" spans="1:99" s="337" customFormat="1">
+    <row r="22" spans="1:99" s="337" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="80" t="s">
         <v>22</v>
       </c>
@@ -33083,7 +33084,7 @@
       <c r="CP22" s="333"/>
       <c r="CU22" s="333"/>
     </row>
-    <row r="23" spans="1:99" s="337" customFormat="1">
+    <row r="23" spans="1:99" s="337" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="80" t="s">
         <v>23</v>
       </c>
@@ -33115,7 +33116,7 @@
       <c r="CP23" s="333"/>
       <c r="CU23" s="333"/>
     </row>
-    <row r="24" spans="1:99" s="337" customFormat="1">
+    <row r="24" spans="1:99" s="337" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="80" t="s">
         <v>26</v>
       </c>
@@ -33142,7 +33143,7 @@
       <c r="CP24" s="333"/>
       <c r="CU24" s="333"/>
     </row>
-    <row r="25" spans="1:99" s="337" customFormat="1">
+    <row r="25" spans="1:99" s="337" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="81" t="s">
         <v>109</v>
       </c>
@@ -33174,7 +33175,7 @@
       <c r="CP25" s="333"/>
       <c r="CU25" s="333"/>
     </row>
-    <row r="26" spans="1:99" s="337" customFormat="1">
+    <row r="26" spans="1:99" s="337" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="81" t="s">
         <v>127</v>
       </c>
@@ -33206,7 +33207,7 @@
       <c r="CP26" s="333"/>
       <c r="CU26" s="333"/>
     </row>
-    <row r="27" spans="1:99" s="337" customFormat="1">
+    <row r="27" spans="1:99" s="337" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="81" t="s">
         <v>128</v>
       </c>
@@ -33240,7 +33241,7 @@
       <c r="CP27" s="333"/>
       <c r="CU27" s="333"/>
     </row>
-    <row r="28" spans="1:99" s="337" customFormat="1">
+    <row r="28" spans="1:99" s="337" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="81" t="s">
         <v>129</v>
       </c>
@@ -33274,7 +33275,7 @@
       <c r="CP28" s="333"/>
       <c r="CU28" s="333"/>
     </row>
-    <row r="29" spans="1:99" s="337" customFormat="1">
+    <row r="29" spans="1:99" s="337" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="81" t="s">
         <v>130</v>
       </c>
@@ -33305,7 +33306,7 @@
       <c r="CP29" s="333"/>
       <c r="CU29" s="333"/>
     </row>
-    <row r="30" spans="1:99" s="337" customFormat="1">
+    <row r="30" spans="1:99" s="337" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="80" t="s">
         <v>20</v>
       </c>
@@ -33333,7 +33334,7 @@
       <c r="CP30" s="333"/>
       <c r="CU30" s="333"/>
     </row>
-    <row r="31" spans="1:99" s="337" customFormat="1">
+    <row r="31" spans="1:99" s="337" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="80" t="s">
         <v>24</v>
       </c>
@@ -33360,7 +33361,7 @@
       <c r="CP31" s="333"/>
       <c r="CU31" s="333"/>
     </row>
-    <row r="32" spans="1:99" s="337" customFormat="1">
+    <row r="32" spans="1:99" s="337" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="80" t="s">
         <v>28</v>
       </c>
@@ -33388,7 +33389,7 @@
       <c r="CP32" s="333"/>
       <c r="CU32" s="333"/>
     </row>
-    <row r="33" spans="1:99" s="365" customFormat="1" ht="15.75" thickBot="1">
+    <row r="33" spans="1:99" s="365" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="124" t="s">
         <v>99</v>
       </c>
@@ -33425,7 +33426,7 @@
       <c r="CP33" s="347"/>
       <c r="CU33" s="347"/>
     </row>
-    <row r="34" spans="1:99" s="367" customFormat="1">
+    <row r="34" spans="1:99" s="367" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="129" t="s">
         <v>97</v>
       </c>
@@ -33452,7 +33453,7 @@
       <c r="CP34" s="344"/>
       <c r="CU34" s="344"/>
     </row>
-    <row r="35" spans="1:99" s="339" customFormat="1">
+    <row r="35" spans="1:99" s="339" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="82" t="s">
         <v>2</v>
       </c>
@@ -33483,7 +33484,7 @@
       <c r="CP35" s="333"/>
       <c r="CU35" s="333"/>
     </row>
-    <row r="36" spans="1:99" s="339" customFormat="1">
+    <row r="36" spans="1:99" s="339" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="82" t="s">
         <v>3</v>
       </c>
@@ -33515,7 +33516,7 @@
       <c r="CP36" s="333"/>
       <c r="CU36" s="333"/>
     </row>
-    <row r="37" spans="1:99" s="339" customFormat="1">
+    <row r="37" spans="1:99" s="339" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="82" t="s">
         <v>1</v>
       </c>
@@ -33546,7 +33547,7 @@
       <c r="CP37" s="333"/>
       <c r="CU37" s="333"/>
     </row>
-    <row r="38" spans="1:99" s="339" customFormat="1">
+    <row r="38" spans="1:99" s="339" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="82" t="s">
         <v>0</v>
       </c>
@@ -33580,7 +33581,7 @@
       <c r="CP38" s="333"/>
       <c r="CU38" s="333"/>
     </row>
-    <row r="39" spans="1:99" s="339" customFormat="1">
+    <row r="39" spans="1:99" s="339" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="172" t="s">
         <v>109</v>
       </c>
@@ -33611,7 +33612,7 @@
       <c r="CP39" s="333"/>
       <c r="CU39" s="333"/>
     </row>
-    <row r="40" spans="1:99" s="339" customFormat="1">
+    <row r="40" spans="1:99" s="339" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="172" t="s">
         <v>127</v>
       </c>
@@ -33641,7 +33642,7 @@
       <c r="CP40" s="333"/>
       <c r="CU40" s="333"/>
     </row>
-    <row r="41" spans="1:99" s="339" customFormat="1">
+    <row r="41" spans="1:99" s="339" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="172" t="s">
         <v>128</v>
       </c>
@@ -33672,7 +33673,7 @@
       <c r="CP41" s="333"/>
       <c r="CU41" s="333"/>
     </row>
-    <row r="42" spans="1:99" s="339" customFormat="1">
+    <row r="42" spans="1:99" s="339" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="172" t="s">
         <v>129</v>
       </c>
@@ -33702,7 +33703,7 @@
       <c r="CP42" s="333"/>
       <c r="CU42" s="333"/>
     </row>
-    <row r="43" spans="1:99" s="339" customFormat="1">
+    <row r="43" spans="1:99" s="339" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="172" t="s">
         <v>130</v>
       </c>
@@ -33733,7 +33734,7 @@
       <c r="CP43" s="333"/>
       <c r="CU43" s="333"/>
     </row>
-    <row r="44" spans="1:99" s="339" customFormat="1">
+    <row r="44" spans="1:99" s="339" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="82" t="s">
         <v>4</v>
       </c>
@@ -33761,7 +33762,7 @@
       <c r="CP44" s="333"/>
       <c r="CU44" s="333"/>
     </row>
-    <row r="45" spans="1:99" s="369" customFormat="1" ht="15.75" thickBot="1">
+    <row r="45" spans="1:99" s="369" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="134" t="s">
         <v>100</v>
       </c>
@@ -33797,7 +33798,7 @@
       <c r="CP45" s="347"/>
       <c r="CU45" s="347"/>
     </row>
-    <row r="46" spans="1:99" s="371" customFormat="1">
+    <row r="46" spans="1:99" s="371" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="139" t="s">
         <v>98</v>
       </c>
@@ -33824,7 +33825,7 @@
       <c r="CP46" s="344"/>
       <c r="CU46" s="344"/>
     </row>
-    <row r="47" spans="1:99" s="340" customFormat="1">
+    <row r="47" spans="1:99" s="340" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="83" t="s">
         <v>29</v>
       </c>
@@ -33855,7 +33856,7 @@
       <c r="CP47" s="333"/>
       <c r="CU47" s="333"/>
     </row>
-    <row r="48" spans="1:99" s="340" customFormat="1">
+    <row r="48" spans="1:99" s="340" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="83" t="s">
         <v>31</v>
       </c>
@@ -33886,7 +33887,7 @@
       <c r="CP48" s="333"/>
       <c r="CU48" s="333"/>
     </row>
-    <row r="49" spans="1:99" s="340" customFormat="1">
+    <row r="49" spans="1:99" s="340" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="83" t="s">
         <v>35</v>
       </c>
@@ -33918,7 +33919,7 @@
       <c r="CP49" s="333"/>
       <c r="CU49" s="333"/>
     </row>
-    <row r="50" spans="1:99" s="340" customFormat="1">
+    <row r="50" spans="1:99" s="340" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="83" t="s">
         <v>30</v>
       </c>
@@ -33949,7 +33950,7 @@
       <c r="CP50" s="333"/>
       <c r="CU50" s="333"/>
     </row>
-    <row r="51" spans="1:99" s="340" customFormat="1">
+    <row r="51" spans="1:99" s="340" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="83" t="s">
         <v>33</v>
       </c>
@@ -33977,7 +33978,7 @@
       <c r="CP51" s="333"/>
       <c r="CU51" s="333"/>
     </row>
-    <row r="52" spans="1:99" s="340" customFormat="1">
+    <row r="52" spans="1:99" s="340" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="83" t="s">
         <v>34</v>
       </c>
@@ -34005,7 +34006,7 @@
       <c r="CP52" s="333"/>
       <c r="CU52" s="333"/>
     </row>
-    <row r="53" spans="1:99" s="340" customFormat="1">
+    <row r="53" spans="1:99" s="340" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="83" t="s">
         <v>32</v>
       </c>
@@ -34033,7 +34034,7 @@
       <c r="CP53" s="333"/>
       <c r="CU53" s="333"/>
     </row>
-    <row r="54" spans="1:99" s="340" customFormat="1">
+    <row r="54" spans="1:99" s="340" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="181" t="s">
         <v>109</v>
       </c>
@@ -34066,7 +34067,7 @@
       <c r="CP54" s="333"/>
       <c r="CU54" s="333"/>
     </row>
-    <row r="55" spans="1:99" s="340" customFormat="1">
+    <row r="55" spans="1:99" s="340" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="181" t="s">
         <v>131</v>
       </c>
@@ -34102,7 +34103,7 @@
       <c r="CP55" s="333"/>
       <c r="CU55" s="333"/>
     </row>
-    <row r="56" spans="1:99" s="340" customFormat="1">
+    <row r="56" spans="1:99" s="340" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="181" t="s">
         <v>132</v>
       </c>
@@ -34136,7 +34137,7 @@
       <c r="CP56" s="333"/>
       <c r="CU56" s="333"/>
     </row>
-    <row r="57" spans="1:99" s="340" customFormat="1">
+    <row r="57" spans="1:99" s="340" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="181" t="s">
         <v>133</v>
       </c>
@@ -34167,7 +34168,7 @@
       <c r="CP57" s="333"/>
       <c r="CU57" s="333"/>
     </row>
-    <row r="58" spans="1:99" s="373" customFormat="1" ht="15.75" thickBot="1">
+    <row r="58" spans="1:99" s="373" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="144" t="s">
         <v>101</v>
       </c>
@@ -34206,7 +34207,7 @@
       <c r="CP58" s="347"/>
       <c r="CU58" s="347"/>
     </row>
-    <row r="59" spans="1:99" s="375" customFormat="1">
+    <row r="59" spans="1:99" s="375" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="154" t="s">
         <v>93</v>
       </c>
@@ -34233,7 +34234,7 @@
       <c r="CP59" s="344"/>
       <c r="CU59" s="344"/>
     </row>
-    <row r="60" spans="1:99" s="341" customFormat="1">
+    <row r="60" spans="1:99" s="341" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="85" t="s">
         <v>5</v>
       </c>
@@ -34262,7 +34263,7 @@
       <c r="CP60" s="333"/>
       <c r="CU60" s="333"/>
     </row>
-    <row r="61" spans="1:99" s="341" customFormat="1">
+    <row r="61" spans="1:99" s="341" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="85" t="s">
         <v>12</v>
       </c>
@@ -34290,7 +34291,7 @@
       <c r="CP61" s="333"/>
       <c r="CU61" s="333"/>
     </row>
-    <row r="62" spans="1:99" s="341" customFormat="1">
+    <row r="62" spans="1:99" s="341" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="84" t="s">
         <v>96</v>
       </c>
@@ -34317,7 +34318,7 @@
       <c r="CP62" s="333"/>
       <c r="CU62" s="333"/>
     </row>
-    <row r="63" spans="1:99" s="341" customFormat="1">
+    <row r="63" spans="1:99" s="341" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="85" t="s">
         <v>25</v>
       </c>
@@ -34346,7 +34347,7 @@
       <c r="CP63" s="333"/>
       <c r="CU63" s="333"/>
     </row>
-    <row r="64" spans="1:99" s="341" customFormat="1">
+    <row r="64" spans="1:99" s="341" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="85" t="s">
         <v>26</v>
       </c>
@@ -34375,7 +34376,7 @@
       <c r="CP64" s="333"/>
       <c r="CU64" s="333"/>
     </row>
-    <row r="65" spans="1:103" s="341" customFormat="1">
+    <row r="65" spans="1:103" s="341" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="84" t="s">
         <v>97</v>
       </c>
@@ -34402,7 +34403,7 @@
       <c r="CP65" s="333"/>
       <c r="CU65" s="333"/>
     </row>
-    <row r="66" spans="1:103" s="341" customFormat="1">
+    <row r="66" spans="1:103" s="341" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="85" t="s">
         <v>0</v>
       </c>
@@ -34431,7 +34432,7 @@
       <c r="CP66" s="333"/>
       <c r="CU66" s="333"/>
     </row>
-    <row r="67" spans="1:103" s="377" customFormat="1" ht="15.75" thickBot="1">
+    <row r="67" spans="1:103" s="377" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="159" t="s">
         <v>102</v>
       </c>
@@ -34464,7 +34465,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="68" spans="1:103" s="382" customFormat="1" ht="15.75" thickBot="1">
+    <row r="68" spans="1:103" s="382" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="210" t="s">
         <v>120</v>
       </c>
@@ -34494,7 +34495,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:103" s="379" customFormat="1">
+    <row r="69" spans="1:103" s="379" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="149"/>
       <c r="B69" s="378"/>
       <c r="C69" s="342"/>
@@ -34529,11 +34530,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E103"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="5.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.5703125" style="414"/>
     <col min="2" max="2" width="5.85546875" style="414" bestFit="1" customWidth="1"/>
@@ -34543,7 +34544,7 @@
     <col min="6" max="16384" width="5.5703125" style="414"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="416" customFormat="1" ht="15.75" thickBot="1">
+    <row r="1" spans="1:5" s="416" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="415"/>
       <c r="B1" s="396" t="s">
         <v>140</v>
@@ -34558,7 +34559,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="417" customFormat="1" ht="45">
+    <row r="2" spans="1:5" s="417" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="471" t="s">
         <v>142</v>
       </c>
@@ -34571,7 +34572,7 @@
       <c r="D2" s="428"/>
       <c r="E2" s="428"/>
     </row>
-    <row r="3" spans="1:5" s="418" customFormat="1">
+    <row r="3" spans="1:5" s="418" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="472"/>
       <c r="B3" s="398">
         <v>43671</v>
@@ -34580,7 +34581,7 @@
       <c r="D3" s="429"/>
       <c r="E3" s="429"/>
     </row>
-    <row r="4" spans="1:5" s="419" customFormat="1" ht="60">
+    <row r="4" spans="1:5" s="419" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="472"/>
       <c r="B4" s="399">
         <v>43672</v>
@@ -34593,7 +34594,7 @@
       </c>
       <c r="E4" s="431"/>
     </row>
-    <row r="5" spans="1:5" s="420" customFormat="1" ht="45">
+    <row r="5" spans="1:5" s="420" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="472"/>
       <c r="B5" s="400">
         <v>43675</v>
@@ -34602,11 +34603,11 @@
         <v>147</v>
       </c>
       <c r="D5" s="433" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E5" s="433"/>
     </row>
-    <row r="6" spans="1:5" s="420" customFormat="1">
+    <row r="6" spans="1:5" s="420" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="472"/>
       <c r="B6" s="400">
         <v>43676</v>
@@ -34619,7 +34620,7 @@
       </c>
       <c r="E6" s="433"/>
     </row>
-    <row r="7" spans="1:5" s="420" customFormat="1" ht="60">
+    <row r="7" spans="1:5" s="420" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="472"/>
       <c r="B7" s="400">
         <v>43677</v>
@@ -34632,7 +34633,7 @@
       </c>
       <c r="E7" s="433"/>
     </row>
-    <row r="8" spans="1:5" s="418" customFormat="1">
+    <row r="8" spans="1:5" s="418" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="472"/>
       <c r="B8" s="398">
         <v>43678</v>
@@ -34641,7 +34642,7 @@
       <c r="D8" s="429"/>
       <c r="E8" s="429"/>
     </row>
-    <row r="9" spans="1:5" s="420" customFormat="1" ht="45">
+    <row r="9" spans="1:5" s="420" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="472"/>
       <c r="B9" s="400">
         <v>43679</v>
@@ -34654,7 +34655,7 @@
       </c>
       <c r="E9" s="433"/>
     </row>
-    <row r="10" spans="1:5" s="419" customFormat="1" ht="51" customHeight="1">
+    <row r="10" spans="1:5" s="419" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="472"/>
       <c r="B10" s="399">
         <v>43682</v>
@@ -34667,7 +34668,7 @@
       </c>
       <c r="E10" s="431"/>
     </row>
-    <row r="11" spans="1:5" s="419" customFormat="1">
+    <row r="11" spans="1:5" s="419" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="472"/>
       <c r="B11" s="399">
         <v>43683</v>
@@ -34680,7 +34681,7 @@
       </c>
       <c r="E11" s="431"/>
     </row>
-    <row r="12" spans="1:5" s="419" customFormat="1">
+    <row r="12" spans="1:5" s="419" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="472"/>
       <c r="B12" s="399">
         <v>43684</v>
@@ -34693,7 +34694,7 @@
       </c>
       <c r="E12" s="431"/>
     </row>
-    <row r="13" spans="1:5" s="418" customFormat="1">
+    <row r="13" spans="1:5" s="418" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="472"/>
       <c r="B13" s="398">
         <v>43685</v>
@@ -34702,7 +34703,7 @@
       <c r="D13" s="429"/>
       <c r="E13" s="429"/>
     </row>
-    <row r="14" spans="1:5" s="419" customFormat="1">
+    <row r="14" spans="1:5" s="419" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="472"/>
       <c r="B14" s="399">
         <v>43686</v>
@@ -34715,7 +34716,7 @@
       </c>
       <c r="E14" s="431"/>
     </row>
-    <row r="15" spans="1:5" s="420" customFormat="1">
+    <row r="15" spans="1:5" s="420" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="472"/>
       <c r="B15" s="400">
         <v>43689</v>
@@ -34728,7 +34729,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="420" customFormat="1">
+    <row r="16" spans="1:5" s="420" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="472"/>
       <c r="B16" s="400">
         <v>43690</v>
@@ -34739,7 +34740,7 @@
       <c r="D16" s="433"/>
       <c r="E16" s="433"/>
     </row>
-    <row r="17" spans="1:5" s="420" customFormat="1">
+    <row r="17" spans="1:5" s="420" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="472"/>
       <c r="B17" s="400">
         <v>43691</v>
@@ -34750,7 +34751,7 @@
       <c r="D17" s="433"/>
       <c r="E17" s="433"/>
     </row>
-    <row r="18" spans="1:5" s="418" customFormat="1">
+    <row r="18" spans="1:5" s="418" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="472"/>
       <c r="B18" s="398">
         <v>43692</v>
@@ -34759,7 +34760,7 @@
       <c r="D18" s="429"/>
       <c r="E18" s="429"/>
     </row>
-    <row r="19" spans="1:5" s="421" customFormat="1" ht="15.75" thickBot="1">
+    <row r="19" spans="1:5" s="421" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="473"/>
       <c r="B19" s="401">
         <v>43693</v>
@@ -34770,7 +34771,7 @@
       <c r="D19" s="434"/>
       <c r="E19" s="434"/>
     </row>
-    <row r="20" spans="1:5" s="417" customFormat="1" ht="45">
+    <row r="20" spans="1:5" s="417" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="468" t="s">
         <v>143</v>
       </c>
@@ -34785,7 +34786,7 @@
       </c>
       <c r="E20" s="428"/>
     </row>
-    <row r="21" spans="1:5" s="419" customFormat="1" ht="45">
+    <row r="21" spans="1:5" s="419" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="469"/>
       <c r="B21" s="403">
         <v>43697</v>
@@ -34798,7 +34799,7 @@
       </c>
       <c r="E21" s="441"/>
     </row>
-    <row r="22" spans="1:5" s="419" customFormat="1" ht="60">
+    <row r="22" spans="1:5" s="419" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="469"/>
       <c r="B22" s="403">
         <v>43698</v>
@@ -34811,7 +34812,7 @@
       </c>
       <c r="E22" s="431"/>
     </row>
-    <row r="23" spans="1:5" s="418" customFormat="1">
+    <row r="23" spans="1:5" s="418" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="469"/>
       <c r="B23" s="404">
         <v>43699</v>
@@ -34820,7 +34821,7 @@
       <c r="D23" s="429"/>
       <c r="E23" s="429"/>
     </row>
-    <row r="24" spans="1:5" s="419" customFormat="1">
+    <row r="24" spans="1:5" s="419" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="469"/>
       <c r="B24" s="403">
         <v>43700</v>
@@ -34831,7 +34832,7 @@
       </c>
       <c r="E24" s="431"/>
     </row>
-    <row r="25" spans="1:5" s="420" customFormat="1" ht="30">
+    <row r="25" spans="1:5" s="420" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="469"/>
       <c r="B25" s="405">
         <v>43703</v>
@@ -34844,7 +34845,7 @@
       </c>
       <c r="E25" s="433"/>
     </row>
-    <row r="26" spans="1:5" s="420" customFormat="1" ht="30">
+    <row r="26" spans="1:5" s="420" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="469"/>
       <c r="B26" s="405">
         <v>43704</v>
@@ -34857,7 +34858,7 @@
       </c>
       <c r="E26" s="433"/>
     </row>
-    <row r="27" spans="1:5" s="420" customFormat="1" ht="30">
+    <row r="27" spans="1:5" s="420" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="469"/>
       <c r="B27" s="405">
         <v>43705</v>
@@ -34870,7 +34871,7 @@
       </c>
       <c r="E27" s="433"/>
     </row>
-    <row r="28" spans="1:5" s="418" customFormat="1">
+    <row r="28" spans="1:5" s="418" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="469"/>
       <c r="B28" s="404">
         <v>43706</v>
@@ -34879,7 +34880,7 @@
       <c r="D28" s="429"/>
       <c r="E28" s="429"/>
     </row>
-    <row r="29" spans="1:5" s="420" customFormat="1">
+    <row r="29" spans="1:5" s="420" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="469"/>
       <c r="B29" s="405">
         <v>43707</v>
@@ -34890,7 +34891,7 @@
       </c>
       <c r="E29" s="433"/>
     </row>
-    <row r="30" spans="1:5" s="419" customFormat="1" ht="45">
+    <row r="30" spans="1:5" s="419" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="469"/>
       <c r="B30" s="403">
         <v>43710</v>
@@ -34901,7 +34902,7 @@
       <c r="D30" s="431"/>
       <c r="E30" s="431"/>
     </row>
-    <row r="31" spans="1:5" s="419" customFormat="1">
+    <row r="31" spans="1:5" s="419" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="469"/>
       <c r="B31" s="403">
         <v>43711</v>
@@ -34912,7 +34913,7 @@
       </c>
       <c r="E31" s="431"/>
     </row>
-    <row r="32" spans="1:5" s="419" customFormat="1">
+    <row r="32" spans="1:5" s="419" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="469"/>
       <c r="B32" s="403">
         <v>43712</v>
@@ -34925,7 +34926,7 @@
       </c>
       <c r="E32" s="431"/>
     </row>
-    <row r="33" spans="1:5" s="418" customFormat="1">
+    <row r="33" spans="1:5" s="418" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="469"/>
       <c r="B33" s="404">
         <v>43713</v>
@@ -34934,7 +34935,7 @@
       <c r="D33" s="429"/>
       <c r="E33" s="429"/>
     </row>
-    <row r="34" spans="1:5" s="419" customFormat="1">
+    <row r="34" spans="1:5" s="419" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="469"/>
       <c r="B34" s="403">
         <v>43714</v>
@@ -34945,7 +34946,7 @@
       <c r="D34" s="431"/>
       <c r="E34" s="431"/>
     </row>
-    <row r="35" spans="1:5" s="420" customFormat="1">
+    <row r="35" spans="1:5" s="420" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="469"/>
       <c r="B35" s="405">
         <v>43717</v>
@@ -34956,7 +34957,7 @@
       <c r="D35" s="433"/>
       <c r="E35" s="433"/>
     </row>
-    <row r="36" spans="1:5" s="420" customFormat="1">
+    <row r="36" spans="1:5" s="420" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="469"/>
       <c r="B36" s="405">
         <v>43718</v>
@@ -34967,7 +34968,7 @@
       <c r="D36" s="433"/>
       <c r="E36" s="433"/>
     </row>
-    <row r="37" spans="1:5" s="420" customFormat="1">
+    <row r="37" spans="1:5" s="420" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="469"/>
       <c r="B37" s="405">
         <v>43719</v>
@@ -34978,7 +34979,7 @@
       <c r="D37" s="433"/>
       <c r="E37" s="433"/>
     </row>
-    <row r="38" spans="1:5" s="418" customFormat="1">
+    <row r="38" spans="1:5" s="418" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="469"/>
       <c r="B38" s="404">
         <v>43720</v>
@@ -34987,7 +34988,7 @@
       <c r="D38" s="429"/>
       <c r="E38" s="429"/>
     </row>
-    <row r="39" spans="1:5" s="420" customFormat="1">
+    <row r="39" spans="1:5" s="420" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="469"/>
       <c r="B39" s="405">
         <v>43721</v>
@@ -34998,7 +34999,7 @@
       <c r="D39" s="433"/>
       <c r="E39" s="433"/>
     </row>
-    <row r="40" spans="1:5" s="419" customFormat="1">
+    <row r="40" spans="1:5" s="419" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="469"/>
       <c r="B40" s="403">
         <v>43724</v>
@@ -35009,7 +35010,7 @@
       <c r="D40" s="431"/>
       <c r="E40" s="431"/>
     </row>
-    <row r="41" spans="1:5" s="419" customFormat="1">
+    <row r="41" spans="1:5" s="419" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="469"/>
       <c r="B41" s="403">
         <v>43725</v>
@@ -35020,7 +35021,7 @@
       <c r="D41" s="431"/>
       <c r="E41" s="431"/>
     </row>
-    <row r="42" spans="1:5" s="419" customFormat="1">
+    <row r="42" spans="1:5" s="419" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="469"/>
       <c r="B42" s="403">
         <v>43726</v>
@@ -35031,7 +35032,7 @@
       <c r="D42" s="431"/>
       <c r="E42" s="431"/>
     </row>
-    <row r="43" spans="1:5" s="418" customFormat="1">
+    <row r="43" spans="1:5" s="418" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="469"/>
       <c r="B43" s="404">
         <v>43727</v>
@@ -35040,7 +35041,7 @@
       <c r="D43" s="429"/>
       <c r="E43" s="429"/>
     </row>
-    <row r="44" spans="1:5" s="422" customFormat="1" ht="15.75" thickBot="1">
+    <row r="44" spans="1:5" s="422" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="470"/>
       <c r="B44" s="406">
         <v>43728</v>
@@ -35051,7 +35052,7 @@
       <c r="D44" s="435"/>
       <c r="E44" s="435"/>
     </row>
-    <row r="45" spans="1:5" s="423" customFormat="1" ht="45">
+    <row r="45" spans="1:5" s="423" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="474" t="s">
         <v>144</v>
       </c>
@@ -35066,7 +35067,7 @@
       </c>
       <c r="E45" s="436"/>
     </row>
-    <row r="46" spans="1:5" s="420" customFormat="1">
+    <row r="46" spans="1:5" s="420" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="475"/>
       <c r="B46" s="408">
         <v>43732</v>
@@ -35079,7 +35080,7 @@
       </c>
       <c r="E46" s="433"/>
     </row>
-    <row r="47" spans="1:5" s="420" customFormat="1" ht="30">
+    <row r="47" spans="1:5" s="420" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="475"/>
       <c r="B47" s="408">
         <v>43733</v>
@@ -35092,7 +35093,7 @@
       </c>
       <c r="E47" s="433"/>
     </row>
-    <row r="48" spans="1:5" s="418" customFormat="1">
+    <row r="48" spans="1:5" s="418" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="475"/>
       <c r="B48" s="409">
         <v>43734</v>
@@ -35101,40 +35102,40 @@
       <c r="D48" s="429"/>
       <c r="E48" s="429"/>
     </row>
-    <row r="49" spans="1:5" s="420" customFormat="1" ht="45">
+    <row r="49" spans="1:5" s="420" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A49" s="475"/>
       <c r="B49" s="408">
         <v>43735</v>
       </c>
       <c r="C49" s="432" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="D49" s="433"/>
       <c r="E49" s="433"/>
     </row>
-    <row r="50" spans="1:5" s="419" customFormat="1" ht="45">
+    <row r="50" spans="1:5" s="419" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="475"/>
       <c r="B50" s="410">
         <v>43738</v>
       </c>
       <c r="C50" s="430" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="D50" s="431"/>
       <c r="E50" s="431"/>
     </row>
-    <row r="51" spans="1:5" s="419" customFormat="1" ht="30">
+    <row r="51" spans="1:5" s="419" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="475"/>
       <c r="B51" s="410">
         <v>43739</v>
       </c>
       <c r="C51" s="430" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D51" s="431"/>
       <c r="E51" s="431"/>
     </row>
-    <row r="52" spans="1:5" s="419" customFormat="1">
+    <row r="52" spans="1:5" s="419" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="475"/>
       <c r="B52" s="410">
         <v>43740</v>
@@ -35145,7 +35146,7 @@
       <c r="D52" s="431"/>
       <c r="E52" s="431"/>
     </row>
-    <row r="53" spans="1:5" s="418" customFormat="1">
+    <row r="53" spans="1:5" s="418" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="475"/>
       <c r="B53" s="409">
         <v>43741</v>
@@ -35154,18 +35155,18 @@
       <c r="D53" s="429"/>
       <c r="E53" s="429"/>
     </row>
-    <row r="54" spans="1:5" s="419" customFormat="1" ht="30">
+    <row r="54" spans="1:5" s="419" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="475"/>
       <c r="B54" s="410">
         <v>43742</v>
       </c>
       <c r="C54" s="430" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D54" s="431"/>
       <c r="E54" s="431"/>
     </row>
-    <row r="55" spans="1:5" s="420" customFormat="1">
+    <row r="55" spans="1:5" s="420" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="475"/>
       <c r="B55" s="408">
         <v>43745</v>
@@ -35176,7 +35177,7 @@
       <c r="D55" s="433"/>
       <c r="E55" s="433"/>
     </row>
-    <row r="56" spans="1:5" s="420" customFormat="1">
+    <row r="56" spans="1:5" s="420" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="475"/>
       <c r="B56" s="408">
         <v>43746</v>
@@ -35187,7 +35188,7 @@
       <c r="D56" s="433"/>
       <c r="E56" s="433"/>
     </row>
-    <row r="57" spans="1:5" s="420" customFormat="1">
+    <row r="57" spans="1:5" s="420" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="475"/>
       <c r="B57" s="408">
         <v>43747</v>
@@ -35198,7 +35199,7 @@
       <c r="D57" s="433"/>
       <c r="E57" s="433"/>
     </row>
-    <row r="58" spans="1:5" s="418" customFormat="1">
+    <row r="58" spans="1:5" s="418" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="475"/>
       <c r="B58" s="409">
         <v>43748</v>
@@ -35207,7 +35208,7 @@
       <c r="D58" s="429"/>
       <c r="E58" s="429"/>
     </row>
-    <row r="59" spans="1:5" s="420" customFormat="1">
+    <row r="59" spans="1:5" s="420" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="475"/>
       <c r="B59" s="408">
         <v>43749</v>
@@ -35218,7 +35219,7 @@
       <c r="D59" s="433"/>
       <c r="E59" s="433"/>
     </row>
-    <row r="60" spans="1:5" s="419" customFormat="1">
+    <row r="60" spans="1:5" s="419" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="475"/>
       <c r="B60" s="410">
         <v>43754</v>
@@ -35229,7 +35230,7 @@
       <c r="D60" s="431"/>
       <c r="E60" s="431"/>
     </row>
-    <row r="61" spans="1:5" s="418" customFormat="1">
+    <row r="61" spans="1:5" s="418" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="475"/>
       <c r="B61" s="409">
         <v>43755</v>
@@ -35238,7 +35239,7 @@
       <c r="D61" s="429"/>
       <c r="E61" s="429"/>
     </row>
-    <row r="62" spans="1:5" s="419" customFormat="1">
+    <row r="62" spans="1:5" s="419" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="475"/>
       <c r="B62" s="410">
         <v>43756</v>
@@ -35249,7 +35250,7 @@
       <c r="D62" s="431"/>
       <c r="E62" s="431"/>
     </row>
-    <row r="63" spans="1:5" s="420" customFormat="1">
+    <row r="63" spans="1:5" s="420" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="475"/>
       <c r="B63" s="408">
         <v>43759</v>
@@ -35260,7 +35261,7 @@
       <c r="D63" s="433"/>
       <c r="E63" s="433"/>
     </row>
-    <row r="64" spans="1:5" s="420" customFormat="1">
+    <row r="64" spans="1:5" s="420" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="475"/>
       <c r="B64" s="408">
         <v>43760</v>
@@ -35271,7 +35272,7 @@
       <c r="D64" s="433"/>
       <c r="E64" s="433"/>
     </row>
-    <row r="65" spans="1:5" s="420" customFormat="1">
+    <row r="65" spans="1:5" s="420" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="475"/>
       <c r="B65" s="408">
         <v>43761</v>
@@ -35282,7 +35283,7 @@
       <c r="D65" s="433"/>
       <c r="E65" s="433"/>
     </row>
-    <row r="66" spans="1:5" s="424" customFormat="1" ht="15.75" thickBot="1">
+    <row r="66" spans="1:5" s="424" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="476"/>
       <c r="B66" s="411">
         <v>43762</v>
@@ -35291,7 +35292,7 @@
       <c r="D66" s="437"/>
       <c r="E66" s="437"/>
     </row>
-    <row r="67" spans="1:5" s="423" customFormat="1" ht="60">
+    <row r="67" spans="1:5" s="423" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A67" s="474" t="s">
         <v>145</v>
       </c>
@@ -35304,7 +35305,7 @@
       <c r="D67" s="436"/>
       <c r="E67" s="436"/>
     </row>
-    <row r="68" spans="1:5" s="419" customFormat="1">
+    <row r="68" spans="1:5" s="419" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="475"/>
       <c r="B68" s="410">
         <v>43766</v>
@@ -35317,7 +35318,7 @@
       </c>
       <c r="E68" s="431"/>
     </row>
-    <row r="69" spans="1:5" s="419" customFormat="1">
+    <row r="69" spans="1:5" s="419" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="475"/>
       <c r="B69" s="410">
         <v>43767</v>
@@ -35330,7 +35331,7 @@
       </c>
       <c r="E69" s="431"/>
     </row>
-    <row r="70" spans="1:5" s="419" customFormat="1">
+    <row r="70" spans="1:5" s="419" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="475"/>
       <c r="B70" s="410">
         <v>43768</v>
@@ -35343,7 +35344,7 @@
       </c>
       <c r="E70" s="431"/>
     </row>
-    <row r="71" spans="1:5" s="418" customFormat="1">
+    <row r="71" spans="1:5" s="418" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="475"/>
       <c r="B71" s="409">
         <v>43769</v>
@@ -35352,18 +35353,18 @@
       <c r="D71" s="429"/>
       <c r="E71" s="429"/>
     </row>
-    <row r="72" spans="1:5" s="419" customFormat="1">
+    <row r="72" spans="1:5" s="419" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="475"/>
       <c r="B72" s="410">
         <v>43770</v>
       </c>
       <c r="C72" s="431" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D72" s="431"/>
       <c r="E72" s="431"/>
     </row>
-    <row r="73" spans="1:5" s="420" customFormat="1">
+    <row r="73" spans="1:5" s="420" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="475"/>
       <c r="B73" s="408">
         <v>43773</v>
@@ -35376,7 +35377,7 @@
       </c>
       <c r="E73" s="433"/>
     </row>
-    <row r="74" spans="1:5" s="420" customFormat="1">
+    <row r="74" spans="1:5" s="420" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="475"/>
       <c r="B74" s="408">
         <v>43774</v>
@@ -35389,18 +35390,18 @@
       </c>
       <c r="E74" s="433"/>
     </row>
-    <row r="75" spans="1:5" s="420" customFormat="1">
+    <row r="75" spans="1:5" s="420" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="475"/>
       <c r="B75" s="408">
         <v>43775</v>
       </c>
       <c r="C75" s="433" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D75" s="433"/>
       <c r="E75" s="433"/>
     </row>
-    <row r="76" spans="1:5" s="418" customFormat="1">
+    <row r="76" spans="1:5" s="418" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="475"/>
       <c r="B76" s="409">
         <v>43776</v>
@@ -35409,7 +35410,7 @@
       <c r="D76" s="429"/>
       <c r="E76" s="429"/>
     </row>
-    <row r="77" spans="1:5" s="420" customFormat="1">
+    <row r="77" spans="1:5" s="420" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="475"/>
       <c r="B77" s="408">
         <v>43777</v>
@@ -35420,7 +35421,7 @@
       <c r="D77" s="433"/>
       <c r="E77" s="433"/>
     </row>
-    <row r="78" spans="1:5" s="419" customFormat="1">
+    <row r="78" spans="1:5" s="419" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="475"/>
       <c r="B78" s="410">
         <v>43780</v>
@@ -35431,7 +35432,7 @@
       <c r="D78" s="431"/>
       <c r="E78" s="431"/>
     </row>
-    <row r="79" spans="1:5" s="419" customFormat="1">
+    <row r="79" spans="1:5" s="419" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="475"/>
       <c r="B79" s="410">
         <v>43781</v>
@@ -35442,7 +35443,7 @@
       <c r="D79" s="431"/>
       <c r="E79" s="431"/>
     </row>
-    <row r="80" spans="1:5" s="419" customFormat="1">
+    <row r="80" spans="1:5" s="419" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="475"/>
       <c r="B80" s="410">
         <v>43782</v>
@@ -35453,7 +35454,7 @@
       <c r="D80" s="431"/>
       <c r="E80" s="431"/>
     </row>
-    <row r="81" spans="1:5" s="418" customFormat="1">
+    <row r="81" spans="1:5" s="418" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="475"/>
       <c r="B81" s="409">
         <v>43783</v>
@@ -35462,7 +35463,7 @@
       <c r="D81" s="429"/>
       <c r="E81" s="429"/>
     </row>
-    <row r="82" spans="1:5" s="420" customFormat="1">
+    <row r="82" spans="1:5" s="420" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="475"/>
       <c r="B82" s="408">
         <v>43787</v>
@@ -35473,7 +35474,7 @@
       <c r="D82" s="433"/>
       <c r="E82" s="433"/>
     </row>
-    <row r="83" spans="1:5" s="420" customFormat="1">
+    <row r="83" spans="1:5" s="420" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="475"/>
       <c r="B83" s="408">
         <v>43788</v>
@@ -35484,7 +35485,7 @@
       <c r="D83" s="433"/>
       <c r="E83" s="433"/>
     </row>
-    <row r="84" spans="1:5" s="418" customFormat="1">
+    <row r="84" spans="1:5" s="418" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="475"/>
       <c r="B84" s="409">
         <v>43790</v>
@@ -35493,7 +35494,7 @@
       <c r="D84" s="429"/>
       <c r="E84" s="429"/>
     </row>
-    <row r="85" spans="1:5" s="420" customFormat="1">
+    <row r="85" spans="1:5" s="420" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="475"/>
       <c r="B85" s="408">
         <v>43791</v>
@@ -35504,7 +35505,7 @@
       <c r="D85" s="433"/>
       <c r="E85" s="433"/>
     </row>
-    <row r="86" spans="1:5" s="419" customFormat="1">
+    <row r="86" spans="1:5" s="419" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="475"/>
       <c r="B86" s="410">
         <v>43794</v>
@@ -35515,7 +35516,7 @@
       <c r="D86" s="431"/>
       <c r="E86" s="431"/>
     </row>
-    <row r="87" spans="1:5" s="419" customFormat="1">
+    <row r="87" spans="1:5" s="419" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="475"/>
       <c r="B87" s="410">
         <v>43795</v>
@@ -35526,7 +35527,7 @@
       <c r="D87" s="431"/>
       <c r="E87" s="431"/>
     </row>
-    <row r="88" spans="1:5" s="419" customFormat="1">
+    <row r="88" spans="1:5" s="419" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="475"/>
       <c r="B88" s="410">
         <v>43796</v>
@@ -35537,7 +35538,7 @@
       <c r="D88" s="431"/>
       <c r="E88" s="431"/>
     </row>
-    <row r="89" spans="1:5" s="424" customFormat="1" ht="15.75" thickBot="1">
+    <row r="89" spans="1:5" s="424" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="476"/>
       <c r="B89" s="411">
         <v>43797</v>
@@ -35546,7 +35547,7 @@
       <c r="D89" s="437"/>
       <c r="E89" s="437"/>
     </row>
-    <row r="90" spans="1:5" s="417" customFormat="1" ht="30">
+    <row r="90" spans="1:5" s="417" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A90" s="468" t="s">
         <v>146</v>
       </c>
@@ -35559,7 +35560,7 @@
       <c r="D90" s="428"/>
       <c r="E90" s="428"/>
     </row>
-    <row r="91" spans="1:5" s="420" customFormat="1">
+    <row r="91" spans="1:5" s="420" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="469"/>
       <c r="B91" s="408">
         <v>43801</v>
@@ -35570,7 +35571,7 @@
       <c r="D91" s="433"/>
       <c r="E91" s="433"/>
     </row>
-    <row r="92" spans="1:5" s="420" customFormat="1">
+    <row r="92" spans="1:5" s="420" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="469"/>
       <c r="B92" s="408">
         <v>43802</v>
@@ -35581,7 +35582,7 @@
       <c r="D92" s="433"/>
       <c r="E92" s="433"/>
     </row>
-    <row r="93" spans="1:5" s="420" customFormat="1">
+    <row r="93" spans="1:5" s="420" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="469"/>
       <c r="B93" s="408">
         <v>43803</v>
@@ -35592,7 +35593,7 @@
       <c r="D93" s="433"/>
       <c r="E93" s="433"/>
     </row>
-    <row r="94" spans="1:5" s="418" customFormat="1">
+    <row r="94" spans="1:5" s="418" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="469"/>
       <c r="B94" s="409">
         <v>43804</v>
@@ -35601,7 +35602,7 @@
       <c r="D94" s="429"/>
       <c r="E94" s="429"/>
     </row>
-    <row r="95" spans="1:5" s="420" customFormat="1">
+    <row r="95" spans="1:5" s="420" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="469"/>
       <c r="B95" s="408">
         <v>43805</v>
@@ -35612,7 +35613,7 @@
       <c r="D95" s="433"/>
       <c r="E95" s="433"/>
     </row>
-    <row r="96" spans="1:5" s="419" customFormat="1">
+    <row r="96" spans="1:5" s="419" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="469"/>
       <c r="B96" s="410">
         <v>43808</v>
@@ -35623,7 +35624,7 @@
       <c r="D96" s="431"/>
       <c r="E96" s="431"/>
     </row>
-    <row r="97" spans="1:5" s="419" customFormat="1">
+    <row r="97" spans="1:5" s="419" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="469"/>
       <c r="B97" s="410">
         <v>43809</v>
@@ -35634,7 +35635,7 @@
       <c r="D97" s="431"/>
       <c r="E97" s="431"/>
     </row>
-    <row r="98" spans="1:5" s="419" customFormat="1">
+    <row r="98" spans="1:5" s="419" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="469"/>
       <c r="B98" s="410">
         <v>43810</v>
@@ -35645,7 +35646,7 @@
       <c r="D98" s="431"/>
       <c r="E98" s="431"/>
     </row>
-    <row r="99" spans="1:5" s="424" customFormat="1" ht="15.75" thickBot="1">
+    <row r="99" spans="1:5" s="424" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="470"/>
       <c r="B99" s="411">
         <v>43811</v>
@@ -35654,7 +35655,7 @@
       <c r="D99" s="437"/>
       <c r="E99" s="437"/>
     </row>
-    <row r="100" spans="1:5" s="425" customFormat="1">
+    <row r="100" spans="1:5" s="425" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B100" s="413">
         <v>43812</v>
       </c>
@@ -35662,7 +35663,7 @@
       <c r="D100" s="438"/>
       <c r="E100" s="438"/>
     </row>
-    <row r="101" spans="1:5" s="420" customFormat="1">
+    <row r="101" spans="1:5" s="420" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B101" s="405">
         <v>43815</v>
       </c>
@@ -35670,7 +35671,7 @@
       <c r="D101" s="433"/>
       <c r="E101" s="433"/>
     </row>
-    <row r="102" spans="1:5" s="420" customFormat="1">
+    <row r="102" spans="1:5" s="420" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B102" s="405">
         <v>43816</v>
       </c>
@@ -35678,7 +35679,7 @@
       <c r="D102" s="433"/>
       <c r="E102" s="433"/>
     </row>
-    <row r="103" spans="1:5" s="420" customFormat="1">
+    <row r="103" spans="1:5" s="420" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B103" s="405">
         <v>43817</v>
       </c>

</xml_diff>